<commit_message>
Add More Section Headings
</commit_message>
<xml_diff>
--- a/IndexResults.xlsx
+++ b/IndexResults.xlsx
@@ -5136,28 +5136,28 @@
         <v>1.160170286</v>
       </c>
       <c r="C2" t="n">
-        <v>2.761710166931152</v>
+        <v>3.035971641540527</v>
       </c>
       <c r="D2" t="n">
-        <v>1.601539880931152</v>
+        <v>1.875801355540527</v>
       </c>
       <c r="E2" t="n">
         <v>0.421895549</v>
       </c>
       <c r="F2" t="n">
-        <v>1.735650181770325</v>
+        <v>1.889573097229004</v>
       </c>
       <c r="G2" t="n">
-        <v>1.313754632770325</v>
+        <v>1.467677548229004</v>
       </c>
       <c r="H2" t="n">
         <v>0.166804667</v>
       </c>
       <c r="I2" t="n">
-        <v>0.7169569134712219</v>
+        <v>0.5093469619750977</v>
       </c>
       <c r="J2" t="n">
-        <v>0.550152246471222</v>
+        <v>0.3425422949750977</v>
       </c>
     </row>
     <row r="3">
@@ -5170,28 +5170,28 @@
         <v>5.936486841</v>
       </c>
       <c r="C3" t="n">
-        <v>8.318574905395508</v>
+        <v>7.764360427856445</v>
       </c>
       <c r="D3" t="n">
-        <v>2.382088064395508</v>
+        <v>1.827873586856446</v>
       </c>
       <c r="E3" t="n">
         <v>0.675904574</v>
       </c>
       <c r="F3" t="n">
-        <v>4.149198532104492</v>
+        <v>3.634698629379272</v>
       </c>
       <c r="G3" t="n">
-        <v>3.473293958104492</v>
+        <v>2.958794055379272</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.9873703122138977</v>
+        <v>0.8147715330123901</v>
       </c>
       <c r="J3" t="n">
-        <v>0.9873703122138977</v>
+        <v>0.8147715330123901</v>
       </c>
     </row>
     <row r="4">
@@ -5204,28 +5204,28 @@
         <v>2.546268592</v>
       </c>
       <c r="C4" t="n">
-        <v>2.661058187484741</v>
+        <v>2.843204736709595</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1147895954847411</v>
+        <v>0.2969361447095946</v>
       </c>
       <c r="E4" t="n">
         <v>0.49047412</v>
       </c>
       <c r="F4" t="n">
-        <v>1.694624662399292</v>
+        <v>1.809594750404358</v>
       </c>
       <c r="G4" t="n">
-        <v>1.204150542399292</v>
+        <v>1.319120630404358</v>
       </c>
       <c r="H4" t="n">
         <v>0.521059036</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9133692383766174</v>
+        <v>0.7301504611968994</v>
       </c>
       <c r="J4" t="n">
-        <v>0.3923102023766174</v>
+        <v>0.2090914251968994</v>
       </c>
     </row>
     <row r="5">
@@ -5238,28 +5238,28 @@
         <v>10.66375011</v>
       </c>
       <c r="C5" t="n">
-        <v>4.13227653503418</v>
+        <v>4.065407276153564</v>
       </c>
       <c r="D5" t="n">
-        <v>6.531473574965821</v>
+        <v>6.598342833846436</v>
       </c>
       <c r="E5" t="n">
         <v>5.367750915</v>
       </c>
       <c r="F5" t="n">
-        <v>2.399416446685791</v>
+        <v>2.381070375442505</v>
       </c>
       <c r="G5" t="n">
-        <v>2.968334468314209</v>
+        <v>2.986680539557495</v>
       </c>
       <c r="H5" t="n">
         <v>0.899989776</v>
       </c>
       <c r="I5" t="n">
-        <v>0.6394060254096985</v>
+        <v>0.340738832950592</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2605837505903015</v>
+        <v>0.5592509430494079</v>
       </c>
     </row>
     <row r="6">
@@ -5272,28 +5272,28 @@
         <v>15.57953993</v>
       </c>
       <c r="C6" t="n">
-        <v>4.264983177185059</v>
+        <v>4.231990814208984</v>
       </c>
       <c r="D6" t="n">
-        <v>11.31455675281494</v>
+        <v>11.34754911579101</v>
       </c>
       <c r="E6" t="n">
         <v>7.136655409</v>
       </c>
       <c r="F6" t="n">
-        <v>2.435023307800293</v>
+        <v>2.406908273696899</v>
       </c>
       <c r="G6" t="n">
-        <v>4.701632101199707</v>
+        <v>4.729747135303101</v>
       </c>
       <c r="H6" t="n">
         <v>0.923829666</v>
       </c>
       <c r="I6" t="n">
-        <v>0.5395832061767578</v>
+        <v>0.2422125488519669</v>
       </c>
       <c r="J6" t="n">
-        <v>0.3842464598232422</v>
+        <v>0.6816171171480332</v>
       </c>
     </row>
     <row r="7">
@@ -5306,28 +5306,28 @@
         <v>1.019390288</v>
       </c>
       <c r="C7" t="n">
-        <v>2.907890796661377</v>
+        <v>3.013283014297485</v>
       </c>
       <c r="D7" t="n">
-        <v>1.888500508661377</v>
+        <v>1.993892726297485</v>
       </c>
       <c r="E7" t="n">
         <v>3.481328281</v>
       </c>
       <c r="F7" t="n">
-        <v>1.937569975852966</v>
+        <v>2.123495817184448</v>
       </c>
       <c r="G7" t="n">
-        <v>1.543758305147034</v>
+        <v>1.357832463815552</v>
       </c>
       <c r="H7" t="n">
         <v>0.617193099</v>
       </c>
       <c r="I7" t="n">
-        <v>0.8661555647850037</v>
+        <v>0.5666282176971436</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2489624657850037</v>
+        <v>0.05056488130285641</v>
       </c>
     </row>
     <row r="8">
@@ -5340,28 +5340,28 @@
         <v>18.58728802</v>
       </c>
       <c r="C8" t="n">
-        <v>9.715904235839844</v>
+        <v>8.926012992858887</v>
       </c>
       <c r="D8" t="n">
-        <v>8.871383784160155</v>
+        <v>9.661275027141112</v>
       </c>
       <c r="E8" t="n">
         <v>7.723795356</v>
       </c>
       <c r="F8" t="n">
-        <v>4.965664863586426</v>
+        <v>4.55111026763916</v>
       </c>
       <c r="G8" t="n">
-        <v>2.758130492413574</v>
+        <v>3.17268508836084</v>
       </c>
       <c r="H8" t="n">
         <v>1.139338063</v>
       </c>
       <c r="I8" t="n">
-        <v>0.5832244157791138</v>
+        <v>0.08946964144706726</v>
       </c>
       <c r="J8" t="n">
-        <v>0.5561136472208863</v>
+        <v>1.049868421552933</v>
       </c>
     </row>
     <row r="9">
@@ -5374,28 +5374,28 @@
         <v>6.151374632</v>
       </c>
       <c r="C9" t="n">
-        <v>4.389376640319824</v>
+        <v>4.234931945800781</v>
       </c>
       <c r="D9" t="n">
-        <v>1.761997991680175</v>
+        <v>1.916442686199218</v>
       </c>
       <c r="E9" t="n">
         <v>1.201903721</v>
       </c>
       <c r="F9" t="n">
-        <v>2.588962554931641</v>
+        <v>2.582365274429321</v>
       </c>
       <c r="G9" t="n">
-        <v>1.387058833931641</v>
+        <v>1.380461553429321</v>
       </c>
       <c r="H9" t="n">
         <v>1.487273197</v>
       </c>
       <c r="I9" t="n">
-        <v>1.836103796958923</v>
+        <v>1.758330464363098</v>
       </c>
       <c r="J9" t="n">
-        <v>0.3488305999589234</v>
+        <v>0.2710572673630982</v>
       </c>
     </row>
     <row r="10">
@@ -5408,28 +5408,28 @@
         <v>12.36649696</v>
       </c>
       <c r="C10" t="n">
-        <v>7.126251220703125</v>
+        <v>6.707079887390137</v>
       </c>
       <c r="D10" t="n">
-        <v>5.240245739296874</v>
+        <v>5.659417072609862</v>
       </c>
       <c r="E10" t="n">
         <v>2.524540508</v>
       </c>
       <c r="F10" t="n">
-        <v>3.84226131439209</v>
+        <v>3.584478616714478</v>
       </c>
       <c r="G10" t="n">
-        <v>1.31772080639209</v>
+        <v>1.059938108714478</v>
       </c>
       <c r="H10" t="n">
         <v>1.956480352</v>
       </c>
       <c r="I10" t="n">
-        <v>1.868015885353088</v>
+        <v>1.734049201011658</v>
       </c>
       <c r="J10" t="n">
-        <v>0.08846446664691165</v>
+        <v>0.2224311509883423</v>
       </c>
     </row>
     <row r="11">
@@ -5442,28 +5442,28 @@
         <v>0.974600892</v>
       </c>
       <c r="C11" t="n">
-        <v>2.75774073600769</v>
+        <v>2.985702991485596</v>
       </c>
       <c r="D11" t="n">
-        <v>1.78313984400769</v>
+        <v>2.011102099485596</v>
       </c>
       <c r="E11" t="n">
         <v>0.393635915</v>
       </c>
       <c r="F11" t="n">
-        <v>1.745952725410461</v>
+        <v>1.889833688735962</v>
       </c>
       <c r="G11" t="n">
-        <v>1.352316810410461</v>
+        <v>1.496197773735962</v>
       </c>
       <c r="H11" t="n">
         <v>0.160959039</v>
       </c>
       <c r="I11" t="n">
-        <v>0.7743073105812073</v>
+        <v>0.558558464050293</v>
       </c>
       <c r="J11" t="n">
-        <v>0.6133482715812073</v>
+        <v>0.397599425050293</v>
       </c>
     </row>
     <row r="12">
@@ -5476,28 +5476,28 @@
         <v>0.785805872</v>
       </c>
       <c r="C12" t="n">
-        <v>2.474215507507324</v>
+        <v>2.832234382629395</v>
       </c>
       <c r="D12" t="n">
-        <v>1.688409635507324</v>
+        <v>2.046428510629394</v>
       </c>
       <c r="E12" t="n">
         <v>0.692475215</v>
       </c>
       <c r="F12" t="n">
-        <v>1.628124594688416</v>
+        <v>1.843997359275818</v>
       </c>
       <c r="G12" t="n">
-        <v>0.9356493796884156</v>
+        <v>1.151522144275818</v>
       </c>
       <c r="H12" t="n">
         <v>0.195450855</v>
       </c>
       <c r="I12" t="n">
-        <v>0.7203201651573181</v>
+        <v>0.521807074546814</v>
       </c>
       <c r="J12" t="n">
-        <v>0.5248693101573181</v>
+        <v>0.3263562195468139</v>
       </c>
     </row>
     <row r="13">
@@ -5510,28 +5510,28 @@
         <v>1.0344302</v>
       </c>
       <c r="C13" t="n">
-        <v>2.90733814239502</v>
+        <v>3.100089073181152</v>
       </c>
       <c r="D13" t="n">
-        <v>1.872907942395019</v>
+        <v>2.065658873181152</v>
       </c>
       <c r="E13" t="n">
         <v>3.016436227</v>
       </c>
       <c r="F13" t="n">
-        <v>1.902608036994934</v>
+        <v>2.09514331817627</v>
       </c>
       <c r="G13" t="n">
-        <v>1.113828190005066</v>
+        <v>0.9212929088237303</v>
       </c>
       <c r="H13" t="n">
         <v>0.408449459</v>
       </c>
       <c r="I13" t="n">
-        <v>0.7501155138015747</v>
+        <v>0.4683831632137299</v>
       </c>
       <c r="J13" t="n">
-        <v>0.3416660548015747</v>
+        <v>0.05993370421372984</v>
       </c>
     </row>
     <row r="14">
@@ -5544,28 +5544,28 @@
         <v>61.8038557</v>
       </c>
       <c r="C14" t="n">
-        <v>48.07374572753906</v>
+        <v>46.59523010253906</v>
       </c>
       <c r="D14" t="n">
-        <v>13.73010997246094</v>
+        <v>15.20862559746094</v>
       </c>
       <c r="E14" t="n">
         <v>25.01149768</v>
       </c>
       <c r="F14" t="n">
-        <v>24.44048690795898</v>
+        <v>23.28647232055664</v>
       </c>
       <c r="G14" t="n">
-        <v>0.5710107720410171</v>
+        <v>1.725025359443361</v>
       </c>
       <c r="H14" t="n">
         <v>3.730481208</v>
       </c>
       <c r="I14" t="n">
-        <v>3.684933423995972</v>
+        <v>1.656699299812317</v>
       </c>
       <c r="J14" t="n">
-        <v>0.04554778400402837</v>
+        <v>2.073781908187683</v>
       </c>
     </row>
     <row r="15">
@@ -5578,28 +5578,28 @@
         <v>2.518653476</v>
       </c>
       <c r="C15" t="n">
-        <v>2.737678050994873</v>
+        <v>2.906314373016357</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2190245749948732</v>
+        <v>0.3876608970163575</v>
       </c>
       <c r="E15" t="n">
         <v>0.66817386</v>
       </c>
       <c r="F15" t="n">
-        <v>1.7371666431427</v>
+        <v>1.851216912269592</v>
       </c>
       <c r="G15" t="n">
-        <v>1.0689927831427</v>
+        <v>1.183043052269592</v>
       </c>
       <c r="H15" t="n">
         <v>0.5032910390000001</v>
       </c>
       <c r="I15" t="n">
-        <v>0.8942362666130066</v>
+        <v>0.6984462738037109</v>
       </c>
       <c r="J15" t="n">
-        <v>0.3909452276130065</v>
+        <v>0.1951552348037109</v>
       </c>
     </row>
     <row r="16">
@@ -5612,28 +5612,28 @@
         <v>1.006196007</v>
       </c>
       <c r="C16" t="n">
-        <v>2.787344694137573</v>
+        <v>3.055233478546143</v>
       </c>
       <c r="D16" t="n">
-        <v>1.781148687137573</v>
+        <v>2.049037471546143</v>
       </c>
       <c r="E16" t="n">
         <v>0.464787932</v>
       </c>
       <c r="F16" t="n">
-        <v>1.752798914909363</v>
+        <v>1.907571911811829</v>
       </c>
       <c r="G16" t="n">
-        <v>1.288010982909363</v>
+        <v>1.442783979811828</v>
       </c>
       <c r="H16" t="n">
         <v>0.186124482</v>
       </c>
       <c r="I16" t="n">
-        <v>0.7137766480445862</v>
+        <v>0.500950813293457</v>
       </c>
       <c r="J16" t="n">
-        <v>0.5276521660445862</v>
+        <v>0.3148263312934571</v>
       </c>
     </row>
     <row r="17">
@@ -5646,28 +5646,28 @@
         <v>2.380706892</v>
       </c>
       <c r="C17" t="n">
-        <v>2.881857633590698</v>
+        <v>2.923670291900635</v>
       </c>
       <c r="D17" t="n">
-        <v>0.5011507415906982</v>
+        <v>0.5429633999006347</v>
       </c>
       <c r="E17" t="n">
         <v>1.708296635</v>
       </c>
       <c r="F17" t="n">
-        <v>1.911916613578796</v>
+        <v>2.046664237976074</v>
       </c>
       <c r="G17" t="n">
-        <v>0.2036199785787964</v>
+        <v>0.3383676029760743</v>
       </c>
       <c r="H17" t="n">
         <v>0.8350595240000001</v>
       </c>
       <c r="I17" t="n">
-        <v>1.172721266746521</v>
+        <v>0.9568867683410645</v>
       </c>
       <c r="J17" t="n">
-        <v>0.3376617427465209</v>
+        <v>0.1218272443410644</v>
       </c>
     </row>
     <row r="18">
@@ -5680,28 +5680,28 @@
         <v>1.78069478</v>
       </c>
       <c r="C18" t="n">
-        <v>3.530785799026489</v>
+        <v>3.60446310043335</v>
       </c>
       <c r="D18" t="n">
-        <v>1.750091019026489</v>
+        <v>1.82376832043335</v>
       </c>
       <c r="E18" t="n">
         <v>0.505519908</v>
       </c>
       <c r="F18" t="n">
-        <v>2.077642917633057</v>
+        <v>2.099247694015503</v>
       </c>
       <c r="G18" t="n">
-        <v>1.572123009633057</v>
+        <v>1.593727786015503</v>
       </c>
       <c r="H18" t="n">
         <v>0.176196273</v>
       </c>
       <c r="I18" t="n">
-        <v>0.7071412205696106</v>
+        <v>0.4750446379184723</v>
       </c>
       <c r="J18" t="n">
-        <v>0.5309449475696106</v>
+        <v>0.2988483649184723</v>
       </c>
     </row>
     <row r="19">
@@ -5714,28 +5714,28 @@
         <v>3.711818396</v>
       </c>
       <c r="C19" t="n">
-        <v>4.021617412567139</v>
+        <v>3.729485988616943</v>
       </c>
       <c r="D19" t="n">
-        <v>0.3097990165671387</v>
+        <v>0.0176675926169434</v>
       </c>
       <c r="E19" t="n">
         <v>5.914797556</v>
       </c>
       <c r="F19" t="n">
-        <v>2.75681209564209</v>
+        <v>3.072922706604004</v>
       </c>
       <c r="G19" t="n">
-        <v>3.15798546035791</v>
+        <v>2.841874849395996</v>
       </c>
       <c r="H19" t="n">
         <v>3.160119003</v>
       </c>
       <c r="I19" t="n">
-        <v>2.660654306411743</v>
+        <v>2.573738098144531</v>
       </c>
       <c r="J19" t="n">
-        <v>0.499464696588257</v>
+        <v>0.5863809048554689</v>
       </c>
     </row>
     <row r="20">
@@ -5748,28 +5748,28 @@
         <v>1.10214478</v>
       </c>
       <c r="C20" t="n">
-        <v>3.637675762176514</v>
+        <v>3.675829410552979</v>
       </c>
       <c r="D20" t="n">
-        <v>2.535530982176514</v>
+        <v>2.573684630552979</v>
       </c>
       <c r="E20" t="n">
         <v>0.797685387</v>
       </c>
       <c r="F20" t="n">
-        <v>2.19162130355835</v>
+        <v>2.252356290817261</v>
       </c>
       <c r="G20" t="n">
-        <v>1.39393591655835</v>
+        <v>1.454670903817261</v>
       </c>
       <c r="H20" t="n">
         <v>0.149094864</v>
       </c>
       <c r="I20" t="n">
-        <v>0.6754158139228821</v>
+        <v>0.3852575719356537</v>
       </c>
       <c r="J20" t="n">
-        <v>0.526320949922882</v>
+        <v>0.2361627079356537</v>
       </c>
     </row>
     <row r="21">
@@ -5782,28 +5782,28 @@
         <v>81.05285287</v>
       </c>
       <c r="C21" t="n">
-        <v>76.53546142578125</v>
+        <v>74.14340972900391</v>
       </c>
       <c r="D21" t="n">
-        <v>4.517391444218745</v>
+        <v>6.909443140996089</v>
       </c>
       <c r="E21" t="n">
         <v>35.78282597</v>
       </c>
       <c r="F21" t="n">
-        <v>39.03950119018555</v>
+        <v>37.45560455322266</v>
       </c>
       <c r="G21" t="n">
-        <v>3.256675220185549</v>
+        <v>1.672778583222659</v>
       </c>
       <c r="H21" t="n">
         <v>4.612928547</v>
       </c>
       <c r="I21" t="n">
-        <v>5.778985500335693</v>
+        <v>2.408670663833618</v>
       </c>
       <c r="J21" t="n">
-        <v>1.166056953335693</v>
+        <v>2.204257883166382</v>
       </c>
     </row>
     <row r="22">
@@ -5816,28 +5816,28 @@
         <v>0.469325038</v>
       </c>
       <c r="C22" t="n">
-        <v>2.272838354110718</v>
+        <v>2.3628830909729</v>
       </c>
       <c r="D22" t="n">
-        <v>1.803513316110718</v>
+        <v>1.8935580529729</v>
       </c>
       <c r="E22" t="n">
         <v>0.321616579</v>
       </c>
       <c r="F22" t="n">
-        <v>1.6682368516922</v>
+        <v>1.875877618789673</v>
       </c>
       <c r="G22" t="n">
-        <v>1.3466202726922</v>
+        <v>1.554261039789673</v>
       </c>
       <c r="H22" t="n">
         <v>0.34214243</v>
       </c>
       <c r="I22" t="n">
-        <v>1.572451114654541</v>
+        <v>1.451704144477844</v>
       </c>
       <c r="J22" t="n">
-        <v>1.230308684654541</v>
+        <v>1.109561714477844</v>
       </c>
     </row>
     <row r="23">
@@ -5850,28 +5850,28 @@
         <v>148.5633238</v>
       </c>
       <c r="C23" t="n">
-        <v>158.7060546875</v>
+        <v>153.9537963867188</v>
       </c>
       <c r="D23" t="n">
-        <v>10.14273088749999</v>
+        <v>5.390472586718744</v>
       </c>
       <c r="E23" t="n">
         <v>77.75262948</v>
       </c>
       <c r="F23" t="n">
-        <v>81.87762451171875</v>
+        <v>79.88976287841797</v>
       </c>
       <c r="G23" t="n">
-        <v>4.124995031718754</v>
+        <v>2.137133398417973</v>
       </c>
       <c r="H23" t="n">
         <v>8.3128054</v>
       </c>
       <c r="I23" t="n">
-        <v>12.4525032043457</v>
+        <v>4.58919620513916</v>
       </c>
       <c r="J23" t="n">
-        <v>4.139697804345703</v>
+        <v>3.72360919486084</v>
       </c>
     </row>
     <row r="24">
@@ -5884,28 +5884,28 @@
         <v>2.139793073</v>
       </c>
       <c r="C24" t="n">
-        <v>2.661042928695679</v>
+        <v>2.760966777801514</v>
       </c>
       <c r="D24" t="n">
-        <v>0.5212498556956788</v>
+        <v>0.6211737048015138</v>
       </c>
       <c r="E24" t="n">
         <v>0.635588045</v>
       </c>
       <c r="F24" t="n">
-        <v>1.764781713485718</v>
+        <v>1.88813054561615</v>
       </c>
       <c r="G24" t="n">
-        <v>1.129193668485718</v>
+        <v>1.25254250061615</v>
       </c>
       <c r="H24" t="n">
         <v>0.603471757</v>
       </c>
       <c r="I24" t="n">
-        <v>1.207040190696716</v>
+        <v>1.039048433303833</v>
       </c>
       <c r="J24" t="n">
-        <v>0.6035684336967163</v>
+        <v>0.435576676303833</v>
       </c>
     </row>
     <row r="25">
@@ -5918,28 +5918,28 @@
         <v>22.11509533</v>
       </c>
       <c r="C25" t="n">
-        <v>16.89458465576172</v>
+        <v>15.66946792602539</v>
       </c>
       <c r="D25" t="n">
-        <v>5.22051067423828</v>
+        <v>6.445627403974608</v>
       </c>
       <c r="E25" t="n">
         <v>7.78555279</v>
       </c>
       <c r="F25" t="n">
-        <v>8.377403259277344</v>
+        <v>7.590682506561279</v>
       </c>
       <c r="G25" t="n">
-        <v>0.5918504692773441</v>
+        <v>0.1948702834387204</v>
       </c>
       <c r="H25" t="n">
         <v>1.185972621</v>
       </c>
       <c r="I25" t="n">
-        <v>0.8502839803695679</v>
+        <v>0.1652802526950836</v>
       </c>
       <c r="J25" t="n">
-        <v>0.335688640630432</v>
+        <v>1.020692368304916</v>
       </c>
     </row>
     <row r="26">
@@ -5952,28 +5952,28 @@
         <v>18.64251276</v>
       </c>
       <c r="C26" t="n">
-        <v>8.959884643554688</v>
+        <v>8.289852142333984</v>
       </c>
       <c r="D26" t="n">
-        <v>9.682628116445311</v>
+        <v>10.35266061766601</v>
       </c>
       <c r="E26" t="n">
         <v>5.905318651</v>
       </c>
       <c r="F26" t="n">
-        <v>4.576831817626953</v>
+        <v>4.146126270294189</v>
       </c>
       <c r="G26" t="n">
-        <v>1.328486833373047</v>
+        <v>1.759192380705811</v>
       </c>
       <c r="H26" t="n">
         <v>1.306022159</v>
       </c>
       <c r="I26" t="n">
-        <v>0.7209558486938477</v>
+        <v>0.3362270891666412</v>
       </c>
       <c r="J26" t="n">
-        <v>0.5850663103061524</v>
+        <v>0.9697950698333588</v>
       </c>
     </row>
     <row r="27">
@@ -5986,28 +5986,28 @@
         <v>1.112044379</v>
       </c>
       <c r="C27" t="n">
-        <v>3.182562112808228</v>
+        <v>3.209793090820312</v>
       </c>
       <c r="D27" t="n">
-        <v>2.070517733808227</v>
+        <v>2.097748711820312</v>
       </c>
       <c r="E27" t="n">
         <v>1.472169653</v>
       </c>
       <c r="F27" t="n">
-        <v>2.047421216964722</v>
+        <v>2.178654909133911</v>
       </c>
       <c r="G27" t="n">
-        <v>0.5752515639647218</v>
+        <v>0.7064852561339112</v>
       </c>
       <c r="H27" t="n">
         <v>0.310931952</v>
       </c>
       <c r="I27" t="n">
-        <v>0.8787896633148193</v>
+        <v>0.5825200080871582</v>
       </c>
       <c r="J27" t="n">
-        <v>0.5678577113148193</v>
+        <v>0.2715880560871582</v>
       </c>
     </row>
     <row r="28">
@@ -6020,28 +6020,28 @@
         <v>1.00422288</v>
       </c>
       <c r="C28" t="n">
-        <v>5.010613918304443</v>
+        <v>4.767471790313721</v>
       </c>
       <c r="D28" t="n">
-        <v>4.006391038304443</v>
+        <v>3.763248910313721</v>
       </c>
       <c r="E28" t="n">
         <v>0.86154519</v>
       </c>
       <c r="F28" t="n">
-        <v>2.874365329742432</v>
+        <v>2.824214935302734</v>
       </c>
       <c r="G28" t="n">
-        <v>2.012820139742431</v>
+        <v>1.962669745302734</v>
       </c>
       <c r="H28" t="n">
         <v>0.086345371</v>
       </c>
       <c r="I28" t="n">
-        <v>0.5393688678741455</v>
+        <v>0.1464018523693085</v>
       </c>
       <c r="J28" t="n">
-        <v>0.4530234968741455</v>
+        <v>0.06005648136930847</v>
       </c>
     </row>
     <row r="29">
@@ -6054,28 +6054,28 @@
         <v>8.949079931</v>
       </c>
       <c r="C29" t="n">
-        <v>3.637582540512085</v>
+        <v>3.696052074432373</v>
       </c>
       <c r="D29" t="n">
-        <v>5.311497390487915</v>
+        <v>5.253027856567627</v>
       </c>
       <c r="E29" t="n">
         <v>5.734039206</v>
       </c>
       <c r="F29" t="n">
-        <v>2.180203437805176</v>
+        <v>2.240268468856812</v>
       </c>
       <c r="G29" t="n">
-        <v>3.553835768194824</v>
+        <v>3.493770737143189</v>
       </c>
       <c r="H29" t="n">
         <v>0.847154045</v>
       </c>
       <c r="I29" t="n">
-        <v>0.6478962898254395</v>
+        <v>0.3644398152828217</v>
       </c>
       <c r="J29" t="n">
-        <v>0.1992577551745606</v>
+        <v>0.4827142297171784</v>
       </c>
     </row>
     <row r="30">
@@ -6088,28 +6088,28 @@
         <v>3.861971089</v>
       </c>
       <c r="C30" t="n">
-        <v>5.634063243865967</v>
+        <v>5.359376430511475</v>
       </c>
       <c r="D30" t="n">
-        <v>1.772092154865967</v>
+        <v>1.497405341511475</v>
       </c>
       <c r="E30" t="n">
         <v>2.16573855</v>
       </c>
       <c r="F30" t="n">
-        <v>3.069186687469482</v>
+        <v>2.900048971176147</v>
       </c>
       <c r="G30" t="n">
-        <v>0.9034481374694825</v>
+        <v>0.7343104211761475</v>
       </c>
       <c r="H30" t="n">
         <v>1.026875013</v>
       </c>
       <c r="I30" t="n">
-        <v>0.9349796175956726</v>
+        <v>0.6873917579650879</v>
       </c>
       <c r="J30" t="n">
-        <v>0.09189539540432734</v>
+        <v>0.3394832550349121</v>
       </c>
     </row>
     <row r="31">
@@ -6122,28 +6122,28 @@
         <v>2.694129305</v>
       </c>
       <c r="C31" t="n">
-        <v>6.793090343475342</v>
+        <v>6.203695297241211</v>
       </c>
       <c r="D31" t="n">
-        <v>4.098961038475341</v>
+        <v>3.509565992241211</v>
       </c>
       <c r="E31" t="n">
         <v>8.998579747999999</v>
       </c>
       <c r="F31" t="n">
-        <v>4.22835636138916</v>
+        <v>4.517917156219482</v>
       </c>
       <c r="G31" t="n">
-        <v>4.770223386610839</v>
+        <v>4.480662591780517</v>
       </c>
       <c r="H31" t="n">
         <v>1.07537871</v>
       </c>
       <c r="I31" t="n">
-        <v>1.460177063941956</v>
+        <v>0.8515607118606567</v>
       </c>
       <c r="J31" t="n">
-        <v>0.3847983539419555</v>
+        <v>0.2238179981393433</v>
       </c>
     </row>
     <row r="32">
@@ -6156,28 +6156,28 @@
         <v>9.584904244000001</v>
       </c>
       <c r="C32" t="n">
-        <v>3.370322942733765</v>
+        <v>3.290653705596924</v>
       </c>
       <c r="D32" t="n">
-        <v>6.214581301266236</v>
+        <v>6.294250538403077</v>
       </c>
       <c r="E32" t="n">
         <v>28.10562387</v>
       </c>
       <c r="F32" t="n">
-        <v>2.304643154144287</v>
+        <v>2.533974170684814</v>
       </c>
       <c r="G32" t="n">
-        <v>25.80098071585571</v>
+        <v>25.57164969931518</v>
       </c>
       <c r="H32" t="n">
         <v>7.878814553</v>
       </c>
       <c r="I32" t="n">
-        <v>1.415459871292114</v>
+        <v>1.140129923820496</v>
       </c>
       <c r="J32" t="n">
-        <v>6.463354681707886</v>
+        <v>6.738684629179504</v>
       </c>
     </row>
     <row r="33">
@@ -6190,28 +6190,28 @@
         <v>22.11264958</v>
       </c>
       <c r="C33" t="n">
-        <v>10.32976818084717</v>
+        <v>9.53678035736084</v>
       </c>
       <c r="D33" t="n">
-        <v>11.78288139915283</v>
+        <v>12.57586922263916</v>
       </c>
       <c r="E33" t="n">
         <v>7.102343521</v>
       </c>
       <c r="F33" t="n">
-        <v>5.244025230407715</v>
+        <v>4.721968173980713</v>
       </c>
       <c r="G33" t="n">
-        <v>1.858318290592285</v>
+        <v>2.380375347019287</v>
       </c>
       <c r="H33" t="n">
         <v>1.625014611</v>
       </c>
       <c r="I33" t="n">
-        <v>0.8046647906303406</v>
+        <v>0.368080198764801</v>
       </c>
       <c r="J33" t="n">
-        <v>0.8203498203696595</v>
+        <v>1.256934412235199</v>
       </c>
     </row>
   </sheetData>
@@ -6295,28 +6295,28 @@
         <v>1.160170286</v>
       </c>
       <c r="C2" t="n">
-        <v>1.643923282623291</v>
+        <v>1.71685516834259</v>
       </c>
       <c r="D2" t="n">
-        <v>0.483752996623291</v>
+        <v>0.5566848823425903</v>
       </c>
       <c r="E2" t="n">
         <v>0.421895549</v>
       </c>
       <c r="F2" t="n">
-        <v>1.405514359474182</v>
+        <v>1.080246329307556</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9836188104741821</v>
+        <v>0.6583507803075561</v>
       </c>
       <c r="H2" t="n">
         <v>0.166804667</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1627254337072372</v>
+        <v>0.3020269274711609</v>
       </c>
       <c r="J2" t="n">
-        <v>0.004079233292762746</v>
+        <v>0.1352222604711609</v>
       </c>
     </row>
     <row r="3">
@@ -6329,28 +6329,28 @@
         <v>5.936486841</v>
       </c>
       <c r="C3" t="n">
-        <v>11.58598709106445</v>
+        <v>11.95135974884033</v>
       </c>
       <c r="D3" t="n">
-        <v>5.649500250064453</v>
+        <v>6.014872907840332</v>
       </c>
       <c r="E3" t="n">
         <v>0.675904574</v>
       </c>
       <c r="F3" t="n">
-        <v>2.199965715408325</v>
+        <v>2.15087103843689</v>
       </c>
       <c r="G3" t="n">
-        <v>1.524061141408325</v>
+        <v>1.47496646443689</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>1.348795056343079</v>
+        <v>2.052312850952148</v>
       </c>
       <c r="J3" t="n">
-        <v>1.348795056343079</v>
+        <v>2.052312850952148</v>
       </c>
     </row>
     <row r="4">
@@ -6363,28 +6363,28 @@
         <v>2.546268592</v>
       </c>
       <c r="C4" t="n">
-        <v>1.546847939491272</v>
+        <v>1.590012788772583</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9994206525087281</v>
+        <v>0.9562558032274171</v>
       </c>
       <c r="E4" t="n">
         <v>0.49047412</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9783089160919189</v>
+        <v>0.6851937174797058</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4878347960919189</v>
+        <v>0.1947195974797058</v>
       </c>
       <c r="H4" t="n">
         <v>0.521059036</v>
       </c>
       <c r="I4" t="n">
-        <v>0.5291029810905457</v>
+        <v>0.5087978839874268</v>
       </c>
       <c r="J4" t="n">
-        <v>0.008043945090545623</v>
+        <v>0.01226115201257327</v>
       </c>
     </row>
     <row r="5">
@@ -6397,28 +6397,28 @@
         <v>10.66375011</v>
       </c>
       <c r="C5" t="n">
-        <v>3.979392290115356</v>
+        <v>3.480880975723267</v>
       </c>
       <c r="D5" t="n">
-        <v>6.684357819884644</v>
+        <v>7.182869134276734</v>
       </c>
       <c r="E5" t="n">
         <v>5.367750915</v>
       </c>
       <c r="F5" t="n">
-        <v>2.944733142852783</v>
+        <v>2.3523850440979</v>
       </c>
       <c r="G5" t="n">
-        <v>2.423017772147217</v>
+        <v>3.0153658709021</v>
       </c>
       <c r="H5" t="n">
         <v>0.899989776</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1543428748846054</v>
+        <v>0.2386967390775681</v>
       </c>
       <c r="J5" t="n">
-        <v>0.7456469011153946</v>
+        <v>0.6612930369224319</v>
       </c>
     </row>
     <row r="6">
@@ -6431,28 +6431,28 @@
         <v>15.57953993</v>
       </c>
       <c r="C6" t="n">
-        <v>4.23035717010498</v>
+        <v>3.64106011390686</v>
       </c>
       <c r="D6" t="n">
-        <v>11.34918275989502</v>
+        <v>11.93847981609314</v>
       </c>
       <c r="E6" t="n">
         <v>7.136655409</v>
       </c>
       <c r="F6" t="n">
-        <v>2.891024827957153</v>
+        <v>2.30732798576355</v>
       </c>
       <c r="G6" t="n">
-        <v>4.245630581042847</v>
+        <v>4.82932742323645</v>
       </c>
       <c r="H6" t="n">
         <v>0.923829666</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.01287080347537994</v>
+        <v>0.1031937748193741</v>
       </c>
       <c r="J6" t="n">
-        <v>0.93670046947538</v>
+        <v>0.820635891180626</v>
       </c>
     </row>
     <row r="7">
@@ -6465,28 +6465,28 @@
         <v>1.019390288</v>
       </c>
       <c r="C7" t="n">
-        <v>1.932649731636047</v>
+        <v>2.013847351074219</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9132594436360473</v>
+        <v>0.9944570630742187</v>
       </c>
       <c r="E7" t="n">
         <v>3.481328281</v>
       </c>
       <c r="F7" t="n">
-        <v>3.303617000579834</v>
+        <v>2.919358491897583</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1777112804201662</v>
+        <v>0.5619697891024171</v>
       </c>
       <c r="H7" t="n">
         <v>0.617193099</v>
       </c>
       <c r="I7" t="n">
-        <v>0.5075545310974121</v>
+        <v>0.5008716583251953</v>
       </c>
       <c r="J7" t="n">
-        <v>0.1096385679025879</v>
+        <v>0.1163214406748047</v>
       </c>
     </row>
     <row r="8">
@@ -6499,28 +6499,28 @@
         <v>18.58728802</v>
       </c>
       <c r="C8" t="n">
-        <v>15.05831146240234</v>
+        <v>16.35537910461426</v>
       </c>
       <c r="D8" t="n">
-        <v>3.528976557597655</v>
+        <v>2.231908915385741</v>
       </c>
       <c r="E8" t="n">
         <v>7.723795356</v>
       </c>
       <c r="F8" t="n">
-        <v>6.518694877624512</v>
+        <v>6.601923942565918</v>
       </c>
       <c r="G8" t="n">
-        <v>1.205100478375488</v>
+        <v>1.121871413434082</v>
       </c>
       <c r="H8" t="n">
         <v>1.139338063</v>
       </c>
       <c r="I8" t="n">
-        <v>0.291964054107666</v>
+        <v>0.7546231150627136</v>
       </c>
       <c r="J8" t="n">
-        <v>0.8473740088923341</v>
+        <v>0.3847149479372864</v>
       </c>
     </row>
     <row r="9">
@@ -6533,28 +6533,28 @@
         <v>6.151374632</v>
       </c>
       <c r="C9" t="n">
-        <v>3.898766756057739</v>
+        <v>4.085438251495361</v>
       </c>
       <c r="D9" t="n">
-        <v>2.25260787594226</v>
+        <v>2.065936380504638</v>
       </c>
       <c r="E9" t="n">
         <v>1.201903721</v>
       </c>
       <c r="F9" t="n">
-        <v>1.754676461219788</v>
+        <v>0.7122712731361389</v>
       </c>
       <c r="G9" t="n">
-        <v>0.5527727402197875</v>
+        <v>0.4896324478638612</v>
       </c>
       <c r="H9" t="n">
         <v>1.487273197</v>
       </c>
       <c r="I9" t="n">
-        <v>2.812133312225342</v>
+        <v>2.848731994628906</v>
       </c>
       <c r="J9" t="n">
-        <v>1.324860115225342</v>
+        <v>1.361458797628906</v>
       </c>
     </row>
     <row r="10">
@@ -6567,28 +6567,28 @@
         <v>12.36649696</v>
       </c>
       <c r="C10" t="n">
-        <v>9.02044677734375</v>
+        <v>10.40627384185791</v>
       </c>
       <c r="D10" t="n">
-        <v>3.346050182656249</v>
+        <v>1.960223118142089</v>
       </c>
       <c r="E10" t="n">
         <v>2.524540508</v>
       </c>
       <c r="F10" t="n">
-        <v>2.843713521957397</v>
+        <v>1.978761553764343</v>
       </c>
       <c r="G10" t="n">
-        <v>0.3191730139573976</v>
+        <v>0.5457789542356566</v>
       </c>
       <c r="H10" t="n">
         <v>1.956480352</v>
       </c>
       <c r="I10" t="n">
-        <v>3.036555767059326</v>
+        <v>3.814637660980225</v>
       </c>
       <c r="J10" t="n">
-        <v>1.080075415059326</v>
+        <v>1.858157308980225</v>
       </c>
     </row>
     <row r="11">
@@ -6601,28 +6601,28 @@
         <v>0.974600892</v>
       </c>
       <c r="C11" t="n">
-        <v>1.645213484764099</v>
+        <v>1.731987953186035</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6706125927640991</v>
+        <v>0.7573870611860352</v>
       </c>
       <c r="E11" t="n">
         <v>0.393635915</v>
       </c>
       <c r="F11" t="n">
-        <v>1.462982416152954</v>
+        <v>1.130110025405884</v>
       </c>
       <c r="G11" t="n">
-        <v>1.069346501152954</v>
+        <v>0.7364741104058838</v>
       </c>
       <c r="H11" t="n">
         <v>0.160959039</v>
       </c>
       <c r="I11" t="n">
-        <v>0.2543874979019165</v>
+        <v>0.3677033185958862</v>
       </c>
       <c r="J11" t="n">
-        <v>0.09342845890191651</v>
+        <v>0.2067442795958862</v>
       </c>
     </row>
     <row r="12">
@@ -6635,28 +6635,28 @@
         <v>0.785805872</v>
       </c>
       <c r="C12" t="n">
-        <v>1.207472920417786</v>
+        <v>1.444767117500305</v>
       </c>
       <c r="D12" t="n">
-        <v>0.4216670484177857</v>
+        <v>0.6589612455003052</v>
       </c>
       <c r="E12" t="n">
         <v>0.692475215</v>
       </c>
       <c r="F12" t="n">
-        <v>1.50673520565033</v>
+        <v>1.21329391002655</v>
       </c>
       <c r="G12" t="n">
-        <v>0.8142599906503296</v>
+        <v>0.5208186950265503</v>
       </c>
       <c r="H12" t="n">
         <v>0.195450855</v>
       </c>
       <c r="I12" t="n">
-        <v>0.1070841997861862</v>
+        <v>0.3128553628921509</v>
       </c>
       <c r="J12" t="n">
-        <v>0.08836665521381379</v>
+        <v>0.1174045078921509</v>
       </c>
     </row>
     <row r="13">
@@ -6669,28 +6669,28 @@
         <v>1.0344302</v>
       </c>
       <c r="C13" t="n">
-        <v>1.942900776863098</v>
+        <v>2.025751352310181</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9084705768630981</v>
+        <v>0.9913211523101806</v>
       </c>
       <c r="E13" t="n">
         <v>3.016436227</v>
       </c>
       <c r="F13" t="n">
-        <v>2.938977241516113</v>
+        <v>2.585455894470215</v>
       </c>
       <c r="G13" t="n">
-        <v>0.07745898548388652</v>
+        <v>0.430980332529785</v>
       </c>
       <c r="H13" t="n">
         <v>0.408449459</v>
       </c>
       <c r="I13" t="n">
-        <v>0.2233205288648605</v>
+        <v>0.3083294034004211</v>
       </c>
       <c r="J13" t="n">
-        <v>0.1851289301351395</v>
+        <v>0.1001200555995789</v>
       </c>
     </row>
     <row r="14">
@@ -6703,28 +6703,28 @@
         <v>61.8038557</v>
       </c>
       <c r="C14" t="n">
-        <v>51.03729629516602</v>
+        <v>57.56928253173828</v>
       </c>
       <c r="D14" t="n">
-        <v>10.76655940483398</v>
+        <v>4.234573168261718</v>
       </c>
       <c r="E14" t="n">
         <v>25.01149768</v>
       </c>
       <c r="F14" t="n">
-        <v>19.89897727966309</v>
+        <v>21.89504623413086</v>
       </c>
       <c r="G14" t="n">
-        <v>5.112520400336916</v>
+        <v>3.116451445869142</v>
       </c>
       <c r="H14" t="n">
         <v>3.730481208</v>
       </c>
       <c r="I14" t="n">
-        <v>1.898283362388611</v>
+        <v>4.003339767456055</v>
       </c>
       <c r="J14" t="n">
-        <v>1.832197845611389</v>
+        <v>0.2728585594560546</v>
       </c>
     </row>
     <row r="15">
@@ -6737,28 +6737,28 @@
         <v>2.518653476</v>
       </c>
       <c r="C15" t="n">
-        <v>1.651172995567322</v>
+        <v>1.690682172775269</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8674804804326781</v>
+        <v>0.8279713032247313</v>
       </c>
       <c r="E15" t="n">
         <v>0.66817386</v>
       </c>
       <c r="F15" t="n">
-        <v>1.173227071762085</v>
+        <v>0.8464617729187012</v>
       </c>
       <c r="G15" t="n">
-        <v>0.505053211762085</v>
+        <v>0.1782879129187012</v>
       </c>
       <c r="H15" t="n">
         <v>0.5032910390000001</v>
       </c>
       <c r="I15" t="n">
-        <v>0.4959650635719299</v>
+        <v>0.4966763854026794</v>
       </c>
       <c r="J15" t="n">
-        <v>0.007325975428070119</v>
+        <v>0.006614653597320608</v>
       </c>
     </row>
     <row r="16">
@@ -6771,28 +6771,28 @@
         <v>1.006196007</v>
       </c>
       <c r="C16" t="n">
-        <v>1.689183235168457</v>
+        <v>1.754834055900574</v>
       </c>
       <c r="D16" t="n">
-        <v>0.682987228168457</v>
+        <v>0.7486380489005737</v>
       </c>
       <c r="E16" t="n">
         <v>0.464787932</v>
       </c>
       <c r="F16" t="n">
-        <v>1.505406260490417</v>
+        <v>1.175041198730469</v>
       </c>
       <c r="G16" t="n">
-        <v>1.040618328490417</v>
+        <v>0.7102532667304687</v>
       </c>
       <c r="H16" t="n">
         <v>0.186124482</v>
       </c>
       <c r="I16" t="n">
-        <v>0.1574511975049973</v>
+        <v>0.2999914884567261</v>
       </c>
       <c r="J16" t="n">
-        <v>0.02867328449500275</v>
+        <v>0.1138670064567261</v>
       </c>
     </row>
     <row r="17">
@@ -6805,28 +6805,28 @@
         <v>2.380706892</v>
       </c>
       <c r="C17" t="n">
-        <v>1.876558899879456</v>
+        <v>1.90115213394165</v>
       </c>
       <c r="D17" t="n">
-        <v>0.5041479921205445</v>
+        <v>0.4795547580583497</v>
       </c>
       <c r="E17" t="n">
         <v>1.708296635</v>
       </c>
       <c r="F17" t="n">
-        <v>2.352059364318848</v>
+        <v>1.771840333938599</v>
       </c>
       <c r="G17" t="n">
-        <v>0.6437627293188477</v>
+        <v>0.06354369893859868</v>
       </c>
       <c r="H17" t="n">
         <v>0.8350595240000001</v>
       </c>
       <c r="I17" t="n">
-        <v>1.170823216438293</v>
+        <v>0.9718776345252991</v>
       </c>
       <c r="J17" t="n">
-        <v>0.3357636924382934</v>
+        <v>0.136818110525299</v>
       </c>
     </row>
     <row r="18">
@@ -6839,28 +6839,28 @@
         <v>1.78069478</v>
       </c>
       <c r="C18" t="n">
-        <v>2.90959620475769</v>
+        <v>2.591815233230591</v>
       </c>
       <c r="D18" t="n">
-        <v>1.128901424757691</v>
+        <v>0.8111204532305909</v>
       </c>
       <c r="E18" t="n">
         <v>0.505519908</v>
       </c>
       <c r="F18" t="n">
-        <v>1.705207943916321</v>
+        <v>1.207934737205505</v>
       </c>
       <c r="G18" t="n">
-        <v>1.199688035916321</v>
+        <v>0.7024148292055054</v>
       </c>
       <c r="H18" t="n">
         <v>0.176196273</v>
       </c>
       <c r="I18" t="n">
-        <v>0.2978107333183289</v>
+        <v>0.3468466997146606</v>
       </c>
       <c r="J18" t="n">
-        <v>0.1216144603183289</v>
+        <v>0.1706504267146607</v>
       </c>
     </row>
     <row r="19">
@@ -6873,28 +6873,28 @@
         <v>3.711818396</v>
       </c>
       <c r="C19" t="n">
-        <v>2.481577396392822</v>
+        <v>3.006704330444336</v>
       </c>
       <c r="D19" t="n">
-        <v>1.230240999607178</v>
+        <v>0.705114065555664</v>
       </c>
       <c r="E19" t="n">
         <v>5.914797556</v>
       </c>
       <c r="F19" t="n">
-        <v>5.740447521209717</v>
+        <v>5.665797233581543</v>
       </c>
       <c r="G19" t="n">
-        <v>0.1743500347902831</v>
+        <v>0.2490003224184569</v>
       </c>
       <c r="H19" t="n">
         <v>3.160119003</v>
       </c>
       <c r="I19" t="n">
-        <v>4.762238502502441</v>
+        <v>5.656315803527832</v>
       </c>
       <c r="J19" t="n">
-        <v>1.602119499502441</v>
+        <v>2.496196800527832</v>
       </c>
     </row>
     <row r="20">
@@ -6907,28 +6907,28 @@
         <v>1.10214478</v>
       </c>
       <c r="C20" t="n">
-        <v>3.156768798828125</v>
+        <v>2.811300992965698</v>
       </c>
       <c r="D20" t="n">
-        <v>2.054624018828125</v>
+        <v>1.709156212965698</v>
       </c>
       <c r="E20" t="n">
         <v>0.797685387</v>
       </c>
       <c r="F20" t="n">
-        <v>2.858088731765747</v>
+        <v>2.353917360305786</v>
       </c>
       <c r="G20" t="n">
-        <v>2.060403344765747</v>
+        <v>1.556231973305786</v>
       </c>
       <c r="H20" t="n">
         <v>0.149094864</v>
       </c>
       <c r="I20" t="n">
-        <v>0.1458070129156113</v>
+        <v>0.2360158115625381</v>
       </c>
       <c r="J20" t="n">
-        <v>0.003287851084388727</v>
+        <v>0.08692094756253815</v>
       </c>
     </row>
     <row r="21">
@@ -6941,28 +6941,28 @@
         <v>81.05285287</v>
       </c>
       <c r="C21" t="n">
-        <v>75.79782867431641</v>
+        <v>86.48673248291016</v>
       </c>
       <c r="D21" t="n">
-        <v>5.255024195683589</v>
+        <v>5.433879612910161</v>
       </c>
       <c r="E21" t="n">
         <v>35.78282597</v>
       </c>
       <c r="F21" t="n">
-        <v>33.53458404541016</v>
+        <v>35.82675170898438</v>
       </c>
       <c r="G21" t="n">
-        <v>2.248241924589841</v>
+        <v>0.04392573898437746</v>
       </c>
       <c r="H21" t="n">
         <v>4.612928547</v>
       </c>
       <c r="I21" t="n">
-        <v>2.639647722244263</v>
+        <v>5.120907783508301</v>
       </c>
       <c r="J21" t="n">
-        <v>1.973280824755737</v>
+        <v>0.5079792365083007</v>
       </c>
     </row>
     <row r="22">
@@ -6975,28 +6975,28 @@
         <v>0.469325038</v>
       </c>
       <c r="C22" t="n">
-        <v>0.9757897257804871</v>
+        <v>1.126173734664917</v>
       </c>
       <c r="D22" t="n">
-        <v>0.506464687780487</v>
+        <v>0.656848696664917</v>
       </c>
       <c r="E22" t="n">
         <v>0.321616579</v>
       </c>
       <c r="F22" t="n">
-        <v>1.814268231391907</v>
+        <v>1.304885149002075</v>
       </c>
       <c r="G22" t="n">
-        <v>1.492651652391907</v>
+        <v>0.9832685700020751</v>
       </c>
       <c r="H22" t="n">
         <v>0.34214243</v>
       </c>
       <c r="I22" t="n">
-        <v>1.941669225692749</v>
+        <v>1.589310765266418</v>
       </c>
       <c r="J22" t="n">
-        <v>1.599526795692749</v>
+        <v>1.247168335266418</v>
       </c>
     </row>
     <row r="23">
@@ -7009,28 +7009,28 @@
         <v>148.5633238</v>
       </c>
       <c r="C23" t="n">
-        <v>142.3776550292969</v>
+        <v>165.0450744628906</v>
       </c>
       <c r="D23" t="n">
-        <v>6.185668770703131</v>
+        <v>16.48175066289062</v>
       </c>
       <c r="E23" t="n">
         <v>77.75262948</v>
       </c>
       <c r="F23" t="n">
-        <v>83.06424713134766</v>
+        <v>84.67376708984375</v>
       </c>
       <c r="G23" t="n">
-        <v>5.31161765134766</v>
+        <v>6.921137609843754</v>
       </c>
       <c r="H23" t="n">
         <v>8.3128054</v>
       </c>
       <c r="I23" t="n">
-        <v>5.823230266571045</v>
+        <v>6.685192584991455</v>
       </c>
       <c r="J23" t="n">
-        <v>2.489575133428955</v>
+        <v>1.627612815008545</v>
       </c>
     </row>
     <row r="24">
@@ -7043,28 +7043,28 @@
         <v>2.139793073</v>
       </c>
       <c r="C24" t="n">
-        <v>1.641902804374695</v>
+        <v>1.645090818405151</v>
       </c>
       <c r="D24" t="n">
-        <v>0.4978902686253051</v>
+        <v>0.4947022545948485</v>
       </c>
       <c r="E24" t="n">
         <v>0.635588045</v>
       </c>
       <c r="F24" t="n">
-        <v>1.380645036697388</v>
+        <v>0.8718785643577576</v>
       </c>
       <c r="G24" t="n">
-        <v>0.7450569916973877</v>
+        <v>0.2362905193577576</v>
       </c>
       <c r="H24" t="n">
         <v>0.603471757</v>
       </c>
       <c r="I24" t="n">
-        <v>1.160987615585327</v>
+        <v>0.9275170564651489</v>
       </c>
       <c r="J24" t="n">
-        <v>0.5575158585853272</v>
+        <v>0.3240452994651489</v>
       </c>
     </row>
     <row r="25">
@@ -7077,28 +7077,28 @@
         <v>22.11509533</v>
       </c>
       <c r="C25" t="n">
-        <v>23.90386962890625</v>
+        <v>26.94645690917969</v>
       </c>
       <c r="D25" t="n">
-        <v>1.788774298906251</v>
+        <v>4.831361579179688</v>
       </c>
       <c r="E25" t="n">
         <v>7.78555279</v>
       </c>
       <c r="F25" t="n">
-        <v>8.046791076660156</v>
+        <v>9.140545845031738</v>
       </c>
       <c r="G25" t="n">
-        <v>0.2612382866601566</v>
+        <v>1.354993055031739</v>
       </c>
       <c r="H25" t="n">
         <v>1.185972621</v>
       </c>
       <c r="I25" t="n">
-        <v>0.5409074425697327</v>
+        <v>1.702297210693359</v>
       </c>
       <c r="J25" t="n">
-        <v>0.6450651784302672</v>
+        <v>0.5163245896933595</v>
       </c>
     </row>
     <row r="26">
@@ -7111,28 +7111,28 @@
         <v>18.64251276</v>
       </c>
       <c r="C26" t="n">
-        <v>13.64951705932617</v>
+        <v>14.53476810455322</v>
       </c>
       <c r="D26" t="n">
-        <v>4.992995700673827</v>
+        <v>4.107744655446776</v>
       </c>
       <c r="E26" t="n">
         <v>5.905318651</v>
       </c>
       <c r="F26" t="n">
-        <v>4.835035800933838</v>
+        <v>4.985452651977539</v>
       </c>
       <c r="G26" t="n">
-        <v>1.070282850066162</v>
+        <v>0.9198659990224609</v>
       </c>
       <c r="H26" t="n">
         <v>1.306022159</v>
       </c>
       <c r="I26" t="n">
-        <v>0.5928405523300171</v>
+        <v>1.08689296245575</v>
       </c>
       <c r="J26" t="n">
-        <v>0.713181606669983</v>
+        <v>0.2191291965442506</v>
       </c>
     </row>
     <row r="27">
@@ -7145,28 +7145,28 @@
         <v>1.112044379</v>
       </c>
       <c r="C27" t="n">
-        <v>2.359725952148438</v>
+        <v>2.293047904968262</v>
       </c>
       <c r="D27" t="n">
-        <v>1.247681573148437</v>
+        <v>1.181003525968262</v>
       </c>
       <c r="E27" t="n">
         <v>1.472169653</v>
       </c>
       <c r="F27" t="n">
-        <v>3.200043916702271</v>
+        <v>2.715330362319946</v>
       </c>
       <c r="G27" t="n">
-        <v>1.727874263702271</v>
+        <v>1.243160709319946</v>
       </c>
       <c r="H27" t="n">
         <v>0.310931952</v>
       </c>
       <c r="I27" t="n">
-        <v>0.5614113807678223</v>
+        <v>0.4963430762290955</v>
       </c>
       <c r="J27" t="n">
-        <v>0.2504794287678223</v>
+        <v>0.1854111242290954</v>
       </c>
     </row>
     <row r="28">
@@ -7179,28 +7179,28 @@
         <v>1.00422288</v>
       </c>
       <c r="C28" t="n">
-        <v>5.655130863189697</v>
+        <v>5.167090892791748</v>
       </c>
       <c r="D28" t="n">
-        <v>4.650907983189697</v>
+        <v>4.162868012791748</v>
       </c>
       <c r="E28" t="n">
         <v>0.86154519</v>
       </c>
       <c r="F28" t="n">
-        <v>4.970434665679932</v>
+        <v>4.611931800842285</v>
       </c>
       <c r="G28" t="n">
-        <v>4.108889475679931</v>
+        <v>3.750386610842285</v>
       </c>
       <c r="H28" t="n">
         <v>0.086345371</v>
       </c>
       <c r="I28" t="n">
-        <v>0.001089528203010559</v>
+        <v>-0.0267719179391861</v>
       </c>
       <c r="J28" t="n">
-        <v>0.08525584279698945</v>
+        <v>0.1131172889391861</v>
       </c>
     </row>
     <row r="29">
@@ -7213,28 +7213,28 @@
         <v>8.949079931</v>
       </c>
       <c r="C29" t="n">
-        <v>3.148920059204102</v>
+        <v>2.794551134109497</v>
       </c>
       <c r="D29" t="n">
-        <v>5.800159871795898</v>
+        <v>6.154528796890503</v>
       </c>
       <c r="E29" t="n">
         <v>5.734039206</v>
       </c>
       <c r="F29" t="n">
-        <v>2.749097108840942</v>
+        <v>2.249882221221924</v>
       </c>
       <c r="G29" t="n">
-        <v>2.984942097159058</v>
+        <v>3.484156984778076</v>
       </c>
       <c r="H29" t="n">
         <v>0.847154045</v>
       </c>
       <c r="I29" t="n">
-        <v>0.104235514998436</v>
+        <v>0.2085471153259277</v>
       </c>
       <c r="J29" t="n">
-        <v>0.742918530001564</v>
+        <v>0.6386069296740723</v>
       </c>
     </row>
     <row r="30">
@@ -7247,28 +7247,28 @@
         <v>3.861971089</v>
       </c>
       <c r="C30" t="n">
-        <v>6.739343166351318</v>
+        <v>6.04601526260376</v>
       </c>
       <c r="D30" t="n">
-        <v>2.877372077351319</v>
+        <v>2.18404417360376</v>
       </c>
       <c r="E30" t="n">
         <v>2.16573855</v>
       </c>
       <c r="F30" t="n">
-        <v>2.75163459777832</v>
+        <v>2.254735946655273</v>
       </c>
       <c r="G30" t="n">
-        <v>0.5858960477783204</v>
+        <v>0.08899739665527351</v>
       </c>
       <c r="H30" t="n">
         <v>1.026875013</v>
       </c>
       <c r="I30" t="n">
-        <v>0.9141685366630554</v>
+        <v>0.9835784435272217</v>
       </c>
       <c r="J30" t="n">
-        <v>0.1127064763369445</v>
+        <v>0.04329656947277827</v>
       </c>
     </row>
     <row r="31">
@@ -7281,28 +7281,28 @@
         <v>2.694129305</v>
       </c>
       <c r="C31" t="n">
-        <v>6.562483310699463</v>
+        <v>7.042696475982666</v>
       </c>
       <c r="D31" t="n">
-        <v>3.868354005699463</v>
+        <v>4.348567170982665</v>
       </c>
       <c r="E31" t="n">
         <v>8.998579747999999</v>
       </c>
       <c r="F31" t="n">
-        <v>12.75977039337158</v>
+        <v>14.48710823059082</v>
       </c>
       <c r="G31" t="n">
-        <v>3.761190645371583</v>
+        <v>5.488528482590821</v>
       </c>
       <c r="H31" t="n">
         <v>1.07537871</v>
       </c>
       <c r="I31" t="n">
-        <v>2.536073684692383</v>
+        <v>2.68515157699585</v>
       </c>
       <c r="J31" t="n">
-        <v>1.460694974692383</v>
+        <v>1.60977286699585</v>
       </c>
     </row>
     <row r="32">
@@ -7315,28 +7315,28 @@
         <v>9.584904244000001</v>
       </c>
       <c r="C32" t="n">
-        <v>2.398838520050049</v>
+        <v>2.217966794967651</v>
       </c>
       <c r="D32" t="n">
-        <v>7.186065723949952</v>
+        <v>7.366937449032349</v>
       </c>
       <c r="E32" t="n">
         <v>28.10562387</v>
       </c>
       <c r="F32" t="n">
-        <v>5.058980941772461</v>
+        <v>4.94398307800293</v>
       </c>
       <c r="G32" t="n">
-        <v>23.04664292822754</v>
+        <v>23.16164079199707</v>
       </c>
       <c r="H32" t="n">
         <v>7.878814553</v>
       </c>
       <c r="I32" t="n">
-        <v>1.910897493362427</v>
+        <v>1.777146816253662</v>
       </c>
       <c r="J32" t="n">
-        <v>5.967917059637573</v>
+        <v>6.101667736746338</v>
       </c>
     </row>
     <row r="33">
@@ -7349,28 +7349,28 @@
         <v>22.11264958</v>
       </c>
       <c r="C33" t="n">
-        <v>16.35378646850586</v>
+        <v>18.12860107421875</v>
       </c>
       <c r="D33" t="n">
-        <v>5.75886311149414</v>
+        <v>3.984048505781249</v>
       </c>
       <c r="E33" t="n">
         <v>7.102343521</v>
       </c>
       <c r="F33" t="n">
-        <v>5.643258571624756</v>
+        <v>5.975821495056152</v>
       </c>
       <c r="G33" t="n">
-        <v>1.459084949375244</v>
+        <v>1.126522025943848</v>
       </c>
       <c r="H33" t="n">
         <v>1.625014611</v>
       </c>
       <c r="I33" t="n">
-        <v>0.7622479200363159</v>
+        <v>1.521459579467773</v>
       </c>
       <c r="J33" t="n">
-        <v>0.8627666909636842</v>
+        <v>0.1035550315322267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Organize Imports, clean up notebook, and get rid of some comments
</commit_message>
<xml_diff>
--- a/IndexResults.xlsx
+++ b/IndexResults.xlsx
@@ -5136,28 +5136,28 @@
         <v>1.160170286</v>
       </c>
       <c r="C2" t="n">
-        <v>3.035971641540527</v>
+        <v>2.770697832107544</v>
       </c>
       <c r="D2" t="n">
-        <v>1.875801355540527</v>
+        <v>1.610527546107544</v>
       </c>
       <c r="E2" t="n">
         <v>0.421895549</v>
       </c>
       <c r="F2" t="n">
-        <v>1.889573097229004</v>
+        <v>1.634085655212402</v>
       </c>
       <c r="G2" t="n">
-        <v>1.467677548229004</v>
+        <v>1.212190106212402</v>
       </c>
       <c r="H2" t="n">
         <v>0.166804667</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5093469619750977</v>
+        <v>0.6188272833824158</v>
       </c>
       <c r="J2" t="n">
-        <v>0.3425422949750977</v>
+        <v>0.4520226163824158</v>
       </c>
     </row>
     <row r="3">
@@ -5170,28 +5170,28 @@
         <v>5.936486841</v>
       </c>
       <c r="C3" t="n">
-        <v>7.764360427856445</v>
+        <v>7.807881832122803</v>
       </c>
       <c r="D3" t="n">
-        <v>1.827873586856446</v>
+        <v>1.871394991122803</v>
       </c>
       <c r="E3" t="n">
         <v>0.675904574</v>
       </c>
       <c r="F3" t="n">
-        <v>3.634698629379272</v>
+        <v>4.036614418029785</v>
       </c>
       <c r="G3" t="n">
-        <v>2.958794055379272</v>
+        <v>3.360709844029785</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8147715330123901</v>
+        <v>0.7153096795082092</v>
       </c>
       <c r="J3" t="n">
-        <v>0.8147715330123901</v>
+        <v>0.7153096795082092</v>
       </c>
     </row>
     <row r="4">
@@ -5204,28 +5204,28 @@
         <v>2.546268592</v>
       </c>
       <c r="C4" t="n">
-        <v>2.843204736709595</v>
+        <v>2.537908315658569</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2969361447095946</v>
+        <v>0.008360276341430772</v>
       </c>
       <c r="E4" t="n">
         <v>0.49047412</v>
       </c>
       <c r="F4" t="n">
-        <v>1.809594750404358</v>
+        <v>1.538327932357788</v>
       </c>
       <c r="G4" t="n">
-        <v>1.319120630404358</v>
+        <v>1.047853812357788</v>
       </c>
       <c r="H4" t="n">
         <v>0.521059036</v>
       </c>
       <c r="I4" t="n">
-        <v>0.7301504611968994</v>
+        <v>0.8021338582038879</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2090914251968994</v>
+        <v>0.2810748222038879</v>
       </c>
     </row>
     <row r="5">
@@ -5238,28 +5238,28 @@
         <v>10.66375011</v>
       </c>
       <c r="C5" t="n">
-        <v>4.065407276153564</v>
+        <v>3.977242469787598</v>
       </c>
       <c r="D5" t="n">
-        <v>6.598342833846436</v>
+        <v>6.686507640212403</v>
       </c>
       <c r="E5" t="n">
         <v>5.367750915</v>
       </c>
       <c r="F5" t="n">
-        <v>2.381070375442505</v>
+        <v>2.273437738418579</v>
       </c>
       <c r="G5" t="n">
-        <v>2.986680539557495</v>
+        <v>3.094313176581421</v>
       </c>
       <c r="H5" t="n">
         <v>0.899989776</v>
       </c>
       <c r="I5" t="n">
-        <v>0.340738832950592</v>
+        <v>0.4547584652900696</v>
       </c>
       <c r="J5" t="n">
-        <v>0.5592509430494079</v>
+        <v>0.4452313107099304</v>
       </c>
     </row>
     <row r="6">
@@ -5272,28 +5272,28 @@
         <v>15.57953993</v>
       </c>
       <c r="C6" t="n">
-        <v>4.231990814208984</v>
+        <v>4.144336700439453</v>
       </c>
       <c r="D6" t="n">
-        <v>11.34754911579101</v>
+        <v>11.43520322956055</v>
       </c>
       <c r="E6" t="n">
         <v>7.136655409</v>
       </c>
       <c r="F6" t="n">
-        <v>2.406908273696899</v>
+        <v>2.313212156295776</v>
       </c>
       <c r="G6" t="n">
-        <v>4.729747135303101</v>
+        <v>4.823443252704224</v>
       </c>
       <c r="H6" t="n">
         <v>0.923829666</v>
       </c>
       <c r="I6" t="n">
-        <v>0.2422125488519669</v>
+        <v>0.3459333777427673</v>
       </c>
       <c r="J6" t="n">
-        <v>0.6816171171480332</v>
+        <v>0.5778962882572327</v>
       </c>
     </row>
     <row r="7">
@@ -5306,28 +5306,28 @@
         <v>1.019390288</v>
       </c>
       <c r="C7" t="n">
-        <v>3.013283014297485</v>
+        <v>2.870755195617676</v>
       </c>
       <c r="D7" t="n">
-        <v>1.993892726297485</v>
+        <v>1.851364907617676</v>
       </c>
       <c r="E7" t="n">
         <v>3.481328281</v>
       </c>
       <c r="F7" t="n">
-        <v>2.123495817184448</v>
+        <v>1.883112549781799</v>
       </c>
       <c r="G7" t="n">
-        <v>1.357832463815552</v>
+        <v>1.598215731218201</v>
       </c>
       <c r="H7" t="n">
         <v>0.617193099</v>
       </c>
       <c r="I7" t="n">
-        <v>0.5666282176971436</v>
+        <v>0.7486581206321716</v>
       </c>
       <c r="J7" t="n">
-        <v>0.05056488130285641</v>
+        <v>0.1314650216321717</v>
       </c>
     </row>
     <row r="8">
@@ -5340,28 +5340,28 @@
         <v>18.58728802</v>
       </c>
       <c r="C8" t="n">
-        <v>8.926012992858887</v>
+        <v>9.289728164672852</v>
       </c>
       <c r="D8" t="n">
-        <v>9.661275027141112</v>
+        <v>9.297559855327147</v>
       </c>
       <c r="E8" t="n">
         <v>7.723795356</v>
       </c>
       <c r="F8" t="n">
-        <v>4.55111026763916</v>
+        <v>5.061763286590576</v>
       </c>
       <c r="G8" t="n">
-        <v>3.17268508836084</v>
+        <v>2.662032069409424</v>
       </c>
       <c r="H8" t="n">
         <v>1.139338063</v>
       </c>
       <c r="I8" t="n">
-        <v>0.08946964144706726</v>
+        <v>0.2974969148635864</v>
       </c>
       <c r="J8" t="n">
-        <v>1.049868421552933</v>
+        <v>0.8418411481364136</v>
       </c>
     </row>
     <row r="9">
@@ -5374,28 +5374,28 @@
         <v>6.151374632</v>
       </c>
       <c r="C9" t="n">
-        <v>4.234931945800781</v>
+        <v>4.11467981338501</v>
       </c>
       <c r="D9" t="n">
-        <v>1.916442686199218</v>
+        <v>2.03669481861499</v>
       </c>
       <c r="E9" t="n">
         <v>1.201903721</v>
       </c>
       <c r="F9" t="n">
-        <v>2.582365274429321</v>
+        <v>2.60042929649353</v>
       </c>
       <c r="G9" t="n">
-        <v>1.380461553429321</v>
+        <v>1.39852557549353</v>
       </c>
       <c r="H9" t="n">
         <v>1.487273197</v>
       </c>
       <c r="I9" t="n">
-        <v>1.758330464363098</v>
+        <v>1.732366442680359</v>
       </c>
       <c r="J9" t="n">
-        <v>0.2710572673630982</v>
+        <v>0.245093245680359</v>
       </c>
     </row>
     <row r="10">
@@ -5408,28 +5408,28 @@
         <v>12.36649696</v>
       </c>
       <c r="C10" t="n">
-        <v>6.707079887390137</v>
+        <v>6.840263843536377</v>
       </c>
       <c r="D10" t="n">
-        <v>5.659417072609862</v>
+        <v>5.526233116463622</v>
       </c>
       <c r="E10" t="n">
         <v>2.524540508</v>
       </c>
       <c r="F10" t="n">
-        <v>3.584478616714478</v>
+        <v>3.933088064193726</v>
       </c>
       <c r="G10" t="n">
-        <v>1.059938108714478</v>
+        <v>1.408547556193726</v>
       </c>
       <c r="H10" t="n">
         <v>1.956480352</v>
       </c>
       <c r="I10" t="n">
-        <v>1.734049201011658</v>
+        <v>1.718608379364014</v>
       </c>
       <c r="J10" t="n">
-        <v>0.2224311509883423</v>
+        <v>0.2378719726359864</v>
       </c>
     </row>
     <row r="11">
@@ -5442,28 +5442,28 @@
         <v>0.974600892</v>
       </c>
       <c r="C11" t="n">
-        <v>2.985702991485596</v>
+        <v>2.723424196243286</v>
       </c>
       <c r="D11" t="n">
-        <v>2.011102099485596</v>
+        <v>1.748823304243286</v>
       </c>
       <c r="E11" t="n">
         <v>0.393635915</v>
       </c>
       <c r="F11" t="n">
-        <v>1.889833688735962</v>
+        <v>1.633400797843933</v>
       </c>
       <c r="G11" t="n">
-        <v>1.496197773735962</v>
+        <v>1.239764882843933</v>
       </c>
       <c r="H11" t="n">
         <v>0.160959039</v>
       </c>
       <c r="I11" t="n">
-        <v>0.558558464050293</v>
+        <v>0.6684341430664062</v>
       </c>
       <c r="J11" t="n">
-        <v>0.397599425050293</v>
+        <v>0.5074751040664063</v>
       </c>
     </row>
     <row r="12">
@@ -5476,28 +5476,28 @@
         <v>0.785805872</v>
       </c>
       <c r="C12" t="n">
-        <v>2.832234382629395</v>
+        <v>2.561013698577881</v>
       </c>
       <c r="D12" t="n">
-        <v>2.046428510629394</v>
+        <v>1.775207826577881</v>
       </c>
       <c r="E12" t="n">
         <v>0.692475215</v>
       </c>
       <c r="F12" t="n">
-        <v>1.843997359275818</v>
+        <v>1.559224247932434</v>
       </c>
       <c r="G12" t="n">
-        <v>1.151522144275818</v>
+        <v>0.8667490329324341</v>
       </c>
       <c r="H12" t="n">
         <v>0.195450855</v>
       </c>
       <c r="I12" t="n">
-        <v>0.521807074546814</v>
+        <v>0.6532016396522522</v>
       </c>
       <c r="J12" t="n">
-        <v>0.3263562195468139</v>
+        <v>0.4577507846522522</v>
       </c>
     </row>
     <row r="13">
@@ -5510,28 +5510,28 @@
         <v>1.0344302</v>
       </c>
       <c r="C13" t="n">
-        <v>3.100089073181152</v>
+        <v>2.931074142456055</v>
       </c>
       <c r="D13" t="n">
-        <v>2.065658873181152</v>
+        <v>1.896643942456055</v>
       </c>
       <c r="E13" t="n">
         <v>3.016436227</v>
       </c>
       <c r="F13" t="n">
-        <v>2.09514331817627</v>
+        <v>1.852902054786682</v>
       </c>
       <c r="G13" t="n">
-        <v>0.9212929088237303</v>
+        <v>1.163534172213318</v>
       </c>
       <c r="H13" t="n">
         <v>0.408449459</v>
       </c>
       <c r="I13" t="n">
-        <v>0.4683831632137299</v>
+        <v>0.6397285461425781</v>
       </c>
       <c r="J13" t="n">
-        <v>0.05993370421372984</v>
+        <v>0.2312790871425781</v>
       </c>
     </row>
     <row r="14">
@@ -5544,28 +5544,28 @@
         <v>61.8038557</v>
       </c>
       <c r="C14" t="n">
-        <v>46.59523010253906</v>
+        <v>46.19211196899414</v>
       </c>
       <c r="D14" t="n">
-        <v>15.20862559746094</v>
+        <v>15.61174373100586</v>
       </c>
       <c r="E14" t="n">
         <v>25.01149768</v>
       </c>
       <c r="F14" t="n">
-        <v>23.28647232055664</v>
+        <v>25.81099128723145</v>
       </c>
       <c r="G14" t="n">
-        <v>1.725025359443361</v>
+        <v>0.7994936072314438</v>
       </c>
       <c r="H14" t="n">
         <v>3.730481208</v>
       </c>
       <c r="I14" t="n">
-        <v>1.656699299812317</v>
+        <v>3.688429832458496</v>
       </c>
       <c r="J14" t="n">
-        <v>2.073781908187683</v>
+        <v>0.04205137554150395</v>
       </c>
     </row>
     <row r="15">
@@ -5578,28 +5578,28 @@
         <v>2.518653476</v>
       </c>
       <c r="C15" t="n">
-        <v>2.906314373016357</v>
+        <v>2.619437217712402</v>
       </c>
       <c r="D15" t="n">
-        <v>0.3876608970163575</v>
+        <v>0.1007837417124025</v>
       </c>
       <c r="E15" t="n">
         <v>0.66817386</v>
       </c>
       <c r="F15" t="n">
-        <v>1.851216912269592</v>
+        <v>1.587683081626892</v>
       </c>
       <c r="G15" t="n">
-        <v>1.183043052269592</v>
+        <v>0.9195092216268921</v>
       </c>
       <c r="H15" t="n">
         <v>0.5032910390000001</v>
       </c>
       <c r="I15" t="n">
-        <v>0.6984462738037109</v>
+        <v>0.7783800959587097</v>
       </c>
       <c r="J15" t="n">
-        <v>0.1951552348037109</v>
+        <v>0.2750890569587097</v>
       </c>
     </row>
     <row r="16">
@@ -5612,28 +5612,28 @@
         <v>1.006196007</v>
       </c>
       <c r="C16" t="n">
-        <v>3.055233478546143</v>
+        <v>2.797711849212646</v>
       </c>
       <c r="D16" t="n">
-        <v>2.049037471546143</v>
+        <v>1.791515842212646</v>
       </c>
       <c r="E16" t="n">
         <v>0.464787932</v>
       </c>
       <c r="F16" t="n">
-        <v>1.907571911811829</v>
+        <v>1.654653429985046</v>
       </c>
       <c r="G16" t="n">
-        <v>1.442783979811828</v>
+        <v>1.189865497985046</v>
       </c>
       <c r="H16" t="n">
         <v>0.186124482</v>
       </c>
       <c r="I16" t="n">
-        <v>0.500950813293457</v>
+        <v>0.6139466166496277</v>
       </c>
       <c r="J16" t="n">
-        <v>0.3148263312934571</v>
+        <v>0.4278221346496277</v>
       </c>
     </row>
     <row r="17">
@@ -5646,28 +5646,28 @@
         <v>2.380706892</v>
       </c>
       <c r="C17" t="n">
-        <v>2.923670291900635</v>
+        <v>2.726659297943115</v>
       </c>
       <c r="D17" t="n">
-        <v>0.5429633999006347</v>
+        <v>0.3459524059431152</v>
       </c>
       <c r="E17" t="n">
         <v>1.708296635</v>
       </c>
       <c r="F17" t="n">
-        <v>2.046664237976074</v>
+        <v>1.827372193336487</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3383676029760743</v>
+        <v>0.1190755583364869</v>
       </c>
       <c r="H17" t="n">
         <v>0.8350595240000001</v>
       </c>
       <c r="I17" t="n">
-        <v>0.9568867683410645</v>
+        <v>1.064384579658508</v>
       </c>
       <c r="J17" t="n">
-        <v>0.1218272443410644</v>
+        <v>0.2293250556585082</v>
       </c>
     </row>
     <row r="18">
@@ -5680,28 +5680,28 @@
         <v>1.78069478</v>
       </c>
       <c r="C18" t="n">
-        <v>3.60446310043335</v>
+        <v>3.397495746612549</v>
       </c>
       <c r="D18" t="n">
-        <v>1.82376832043335</v>
+        <v>1.616800966612549</v>
       </c>
       <c r="E18" t="n">
         <v>0.505519908</v>
       </c>
       <c r="F18" t="n">
-        <v>2.099247694015503</v>
+        <v>1.921924114227295</v>
       </c>
       <c r="G18" t="n">
-        <v>1.593727786015503</v>
+        <v>1.416404206227295</v>
       </c>
       <c r="H18" t="n">
         <v>0.176196273</v>
       </c>
       <c r="I18" t="n">
-        <v>0.4750446379184723</v>
+        <v>0.5488576889038086</v>
       </c>
       <c r="J18" t="n">
-        <v>0.2988483649184723</v>
+        <v>0.3726614159038086</v>
       </c>
     </row>
     <row r="19">
@@ -5714,28 +5714,28 @@
         <v>3.711818396</v>
       </c>
       <c r="C19" t="n">
-        <v>3.729485988616943</v>
+        <v>3.893709182739258</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0176675926169434</v>
+        <v>0.1818907867392578</v>
       </c>
       <c r="E19" t="n">
         <v>5.914797556</v>
       </c>
       <c r="F19" t="n">
-        <v>3.072922706604004</v>
+        <v>3.158528566360474</v>
       </c>
       <c r="G19" t="n">
-        <v>2.841874849395996</v>
+        <v>2.756268989639526</v>
       </c>
       <c r="H19" t="n">
         <v>3.160119003</v>
       </c>
       <c r="I19" t="n">
-        <v>2.573738098144531</v>
+        <v>2.751118898391724</v>
       </c>
       <c r="J19" t="n">
-        <v>0.5863809048554689</v>
+        <v>0.4090001046082765</v>
       </c>
     </row>
     <row r="20">
@@ -5748,28 +5748,28 @@
         <v>1.10214478</v>
       </c>
       <c r="C20" t="n">
-        <v>3.675829410552979</v>
+        <v>3.556252479553223</v>
       </c>
       <c r="D20" t="n">
-        <v>2.573684630552979</v>
+        <v>2.454107699553223</v>
       </c>
       <c r="E20" t="n">
         <v>0.797685387</v>
       </c>
       <c r="F20" t="n">
-        <v>2.252356290817261</v>
+        <v>2.093706130981445</v>
       </c>
       <c r="G20" t="n">
-        <v>1.454670903817261</v>
+        <v>1.296020743981445</v>
       </c>
       <c r="H20" t="n">
         <v>0.149094864</v>
       </c>
       <c r="I20" t="n">
-        <v>0.3852575719356537</v>
+        <v>0.5183082222938538</v>
       </c>
       <c r="J20" t="n">
-        <v>0.2361627079356537</v>
+        <v>0.3692133582938538</v>
       </c>
     </row>
     <row r="21">
@@ -5782,28 +5782,28 @@
         <v>81.05285287</v>
       </c>
       <c r="C21" t="n">
-        <v>74.14340972900391</v>
+        <v>73.70899200439453</v>
       </c>
       <c r="D21" t="n">
-        <v>6.909443140996089</v>
+        <v>7.343860865605464</v>
       </c>
       <c r="E21" t="n">
         <v>35.78282597</v>
       </c>
       <c r="F21" t="n">
-        <v>37.45560455322266</v>
+        <v>41.37599563598633</v>
       </c>
       <c r="G21" t="n">
-        <v>1.672778583222659</v>
+        <v>5.593169665986331</v>
       </c>
       <c r="H21" t="n">
         <v>4.612928547</v>
       </c>
       <c r="I21" t="n">
-        <v>2.408670663833618</v>
+        <v>6.02285099029541</v>
       </c>
       <c r="J21" t="n">
-        <v>2.204257883166382</v>
+        <v>1.40992244329541</v>
       </c>
     </row>
     <row r="22">
@@ -5816,28 +5816,28 @@
         <v>0.469325038</v>
       </c>
       <c r="C22" t="n">
-        <v>2.3628830909729</v>
+        <v>2.087308645248413</v>
       </c>
       <c r="D22" t="n">
-        <v>1.8935580529729</v>
+        <v>1.617983607248413</v>
       </c>
       <c r="E22" t="n">
         <v>0.321616579</v>
       </c>
       <c r="F22" t="n">
-        <v>1.875877618789673</v>
+        <v>1.627632975578308</v>
       </c>
       <c r="G22" t="n">
-        <v>1.554261039789673</v>
+        <v>1.306016396578308</v>
       </c>
       <c r="H22" t="n">
         <v>0.34214243</v>
       </c>
       <c r="I22" t="n">
-        <v>1.451704144477844</v>
+        <v>1.526596665382385</v>
       </c>
       <c r="J22" t="n">
-        <v>1.109561714477844</v>
+        <v>1.184454235382385</v>
       </c>
     </row>
     <row r="23">
@@ -5850,28 +5850,28 @@
         <v>148.5633238</v>
       </c>
       <c r="C23" t="n">
-        <v>153.9537963867188</v>
+        <v>154.4186248779297</v>
       </c>
       <c r="D23" t="n">
-        <v>5.390472586718744</v>
+        <v>5.855301077929681</v>
       </c>
       <c r="E23" t="n">
         <v>77.75262948</v>
       </c>
       <c r="F23" t="n">
-        <v>79.88976287841797</v>
+        <v>87.72187042236328</v>
       </c>
       <c r="G23" t="n">
-        <v>2.137133398417973</v>
+        <v>9.969240942363285</v>
       </c>
       <c r="H23" t="n">
         <v>8.3128054</v>
       </c>
       <c r="I23" t="n">
-        <v>4.58919620513916</v>
+        <v>13.49117374420166</v>
       </c>
       <c r="J23" t="n">
-        <v>3.72360919486084</v>
+        <v>5.17836834420166</v>
       </c>
     </row>
     <row r="24">
@@ -5884,28 +5884,28 @@
         <v>2.139793073</v>
       </c>
       <c r="C24" t="n">
-        <v>2.760966777801514</v>
+        <v>2.487301111221313</v>
       </c>
       <c r="D24" t="n">
-        <v>0.6211737048015138</v>
+        <v>0.3475080382213136</v>
       </c>
       <c r="E24" t="n">
         <v>0.635588045</v>
       </c>
       <c r="F24" t="n">
-        <v>1.88813054561615</v>
+        <v>1.647400379180908</v>
       </c>
       <c r="G24" t="n">
-        <v>1.25254250061615</v>
+        <v>1.011812334180908</v>
       </c>
       <c r="H24" t="n">
         <v>0.603471757</v>
       </c>
       <c r="I24" t="n">
-        <v>1.039048433303833</v>
+        <v>1.10819935798645</v>
       </c>
       <c r="J24" t="n">
-        <v>0.435576676303833</v>
+        <v>0.5047276009864502</v>
       </c>
     </row>
     <row r="25">
@@ -5918,28 +5918,28 @@
         <v>22.11509533</v>
       </c>
       <c r="C25" t="n">
-        <v>15.66946792602539</v>
+        <v>15.55559921264648</v>
       </c>
       <c r="D25" t="n">
-        <v>6.445627403974608</v>
+        <v>6.559496117353515</v>
       </c>
       <c r="E25" t="n">
         <v>7.78555279</v>
       </c>
       <c r="F25" t="n">
-        <v>7.590682506561279</v>
+        <v>8.477485656738281</v>
       </c>
       <c r="G25" t="n">
-        <v>0.1948702834387204</v>
+        <v>0.6919328667382816</v>
       </c>
       <c r="H25" t="n">
         <v>1.185972621</v>
       </c>
       <c r="I25" t="n">
-        <v>0.1652802526950836</v>
+        <v>0.6906794905662537</v>
       </c>
       <c r="J25" t="n">
-        <v>1.020692368304916</v>
+        <v>0.4952931304337462</v>
       </c>
     </row>
     <row r="26">
@@ -5952,28 +5952,28 @@
         <v>18.64251276</v>
       </c>
       <c r="C26" t="n">
-        <v>8.289852142333984</v>
+        <v>8.574667930603027</v>
       </c>
       <c r="D26" t="n">
-        <v>10.35266061766601</v>
+        <v>10.06784482939697</v>
       </c>
       <c r="E26" t="n">
         <v>5.905318651</v>
       </c>
       <c r="F26" t="n">
-        <v>4.146126270294189</v>
+        <v>4.5907883644104</v>
       </c>
       <c r="G26" t="n">
-        <v>1.759192380705811</v>
+        <v>1.3145302865896</v>
       </c>
       <c r="H26" t="n">
         <v>1.306022159</v>
       </c>
       <c r="I26" t="n">
-        <v>0.3362270891666412</v>
+        <v>0.4287429451942444</v>
       </c>
       <c r="J26" t="n">
-        <v>0.9697950698333588</v>
+        <v>0.8772792138057557</v>
       </c>
     </row>
     <row r="27">
@@ -5986,28 +5986,28 @@
         <v>1.112044379</v>
       </c>
       <c r="C27" t="n">
-        <v>3.209793090820312</v>
+        <v>3.084545612335205</v>
       </c>
       <c r="D27" t="n">
-        <v>2.097748711820312</v>
+        <v>1.972501233335205</v>
       </c>
       <c r="E27" t="n">
         <v>1.472169653</v>
       </c>
       <c r="F27" t="n">
-        <v>2.178654909133911</v>
+        <v>1.970826029777527</v>
       </c>
       <c r="G27" t="n">
-        <v>0.7064852561339112</v>
+        <v>0.4986563767775269</v>
       </c>
       <c r="H27" t="n">
         <v>0.310931952</v>
       </c>
       <c r="I27" t="n">
-        <v>0.5825200080871582</v>
+        <v>0.7447643876075745</v>
       </c>
       <c r="J27" t="n">
-        <v>0.2715880560871582</v>
+        <v>0.4338324356075745</v>
       </c>
     </row>
     <row r="28">
@@ -6020,28 +6020,28 @@
         <v>1.00422288</v>
       </c>
       <c r="C28" t="n">
-        <v>4.767471790313721</v>
+        <v>4.857752323150635</v>
       </c>
       <c r="D28" t="n">
-        <v>3.763248910313721</v>
+        <v>3.853529443150635</v>
       </c>
       <c r="E28" t="n">
         <v>0.86154519</v>
       </c>
       <c r="F28" t="n">
-        <v>2.824214935302734</v>
+        <v>2.81243371963501</v>
       </c>
       <c r="G28" t="n">
-        <v>1.962669745302734</v>
+        <v>1.95088852963501</v>
       </c>
       <c r="H28" t="n">
         <v>0.086345371</v>
       </c>
       <c r="I28" t="n">
-        <v>0.1464018523693085</v>
+        <v>0.3160014748573303</v>
       </c>
       <c r="J28" t="n">
-        <v>0.06005648136930847</v>
+        <v>0.2296561038573303</v>
       </c>
     </row>
     <row r="29">
@@ -6054,28 +6054,28 @@
         <v>8.949079931</v>
       </c>
       <c r="C29" t="n">
-        <v>3.696052074432373</v>
+        <v>3.570563793182373</v>
       </c>
       <c r="D29" t="n">
-        <v>5.253027856567627</v>
+        <v>5.378516137817627</v>
       </c>
       <c r="E29" t="n">
         <v>5.734039206</v>
       </c>
       <c r="F29" t="n">
-        <v>2.240268468856812</v>
+        <v>2.082376480102539</v>
       </c>
       <c r="G29" t="n">
-        <v>3.493770737143189</v>
+        <v>3.651662725897461</v>
       </c>
       <c r="H29" t="n">
         <v>0.847154045</v>
       </c>
       <c r="I29" t="n">
-        <v>0.3644398152828217</v>
+        <v>0.49187171459198</v>
       </c>
       <c r="J29" t="n">
-        <v>0.4827142297171784</v>
+        <v>0.35528233040802</v>
       </c>
     </row>
     <row r="30">
@@ -6088,28 +6088,28 @@
         <v>3.861971089</v>
       </c>
       <c r="C30" t="n">
-        <v>5.359376430511475</v>
+        <v>5.327510356903076</v>
       </c>
       <c r="D30" t="n">
-        <v>1.497405341511475</v>
+        <v>1.465539267903076</v>
       </c>
       <c r="E30" t="n">
         <v>2.16573855</v>
       </c>
       <c r="F30" t="n">
-        <v>2.900048971176147</v>
+        <v>2.967047452926636</v>
       </c>
       <c r="G30" t="n">
-        <v>0.7343104211761475</v>
+        <v>0.8013089029266358</v>
       </c>
       <c r="H30" t="n">
         <v>1.026875013</v>
       </c>
       <c r="I30" t="n">
-        <v>0.6873917579650879</v>
+        <v>0.7067816257476807</v>
       </c>
       <c r="J30" t="n">
-        <v>0.3394832550349121</v>
+        <v>0.3200933872523193</v>
       </c>
     </row>
     <row r="31">
@@ -6122,28 +6122,28 @@
         <v>2.694129305</v>
       </c>
       <c r="C31" t="n">
-        <v>6.203695297241211</v>
+        <v>6.865587711334229</v>
       </c>
       <c r="D31" t="n">
-        <v>3.509565992241211</v>
+        <v>4.171458406334228</v>
       </c>
       <c r="E31" t="n">
         <v>8.998579747999999</v>
       </c>
       <c r="F31" t="n">
-        <v>4.517917156219482</v>
+        <v>4.770915508270264</v>
       </c>
       <c r="G31" t="n">
-        <v>4.480662591780517</v>
+        <v>4.227664239729735</v>
       </c>
       <c r="H31" t="n">
         <v>1.07537871</v>
       </c>
       <c r="I31" t="n">
-        <v>0.8515607118606567</v>
+        <v>1.347963571548462</v>
       </c>
       <c r="J31" t="n">
-        <v>0.2238179981393433</v>
+        <v>0.2725848615484618</v>
       </c>
     </row>
     <row r="32">
@@ -6156,28 +6156,28 @@
         <v>9.584904244000001</v>
       </c>
       <c r="C32" t="n">
-        <v>3.290653705596924</v>
+        <v>3.23934531211853</v>
       </c>
       <c r="D32" t="n">
-        <v>6.294250538403077</v>
+        <v>6.34555893188147</v>
       </c>
       <c r="E32" t="n">
         <v>28.10562387</v>
       </c>
       <c r="F32" t="n">
-        <v>2.533974170684814</v>
+        <v>2.389941692352295</v>
       </c>
       <c r="G32" t="n">
-        <v>25.57164969931518</v>
+        <v>25.7156821776477</v>
       </c>
       <c r="H32" t="n">
         <v>7.878814553</v>
       </c>
       <c r="I32" t="n">
-        <v>1.140129923820496</v>
+        <v>1.333219647407532</v>
       </c>
       <c r="J32" t="n">
-        <v>6.738684629179504</v>
+        <v>6.545594905592468</v>
       </c>
     </row>
     <row r="33">
@@ -6190,28 +6190,28 @@
         <v>22.11264958</v>
       </c>
       <c r="C33" t="n">
-        <v>9.53678035736084</v>
+        <v>9.845495223999023</v>
       </c>
       <c r="D33" t="n">
-        <v>12.57586922263916</v>
+        <v>12.26715435600098</v>
       </c>
       <c r="E33" t="n">
         <v>7.102343521</v>
       </c>
       <c r="F33" t="n">
-        <v>4.721968173980713</v>
+        <v>5.344236850738525</v>
       </c>
       <c r="G33" t="n">
-        <v>2.380375347019287</v>
+        <v>1.758106670261474</v>
       </c>
       <c r="H33" t="n">
         <v>1.625014611</v>
       </c>
       <c r="I33" t="n">
-        <v>0.368080198764801</v>
+        <v>0.5050948858261108</v>
       </c>
       <c r="J33" t="n">
-        <v>1.256934412235199</v>
+        <v>1.119919725173889</v>
       </c>
     </row>
   </sheetData>
@@ -6295,28 +6295,28 @@
         <v>1.160170286</v>
       </c>
       <c r="C2" t="n">
-        <v>1.71685516834259</v>
+        <v>2.058802366256714</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5566848823425903</v>
+        <v>0.8986320802567138</v>
       </c>
       <c r="E2" t="n">
         <v>0.421895549</v>
       </c>
       <c r="F2" t="n">
-        <v>1.080246329307556</v>
+        <v>1.487817764282227</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6583507803075561</v>
+        <v>1.065922215282227</v>
       </c>
       <c r="H2" t="n">
         <v>0.166804667</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3020269274711609</v>
+        <v>0.3832489252090454</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1352222604711609</v>
+        <v>0.2164442582090454</v>
       </c>
     </row>
     <row r="3">
@@ -6329,28 +6329,28 @@
         <v>5.936486841</v>
       </c>
       <c r="C3" t="n">
-        <v>11.95135974884033</v>
+        <v>11.90138721466064</v>
       </c>
       <c r="D3" t="n">
-        <v>6.014872907840332</v>
+        <v>5.964900373660645</v>
       </c>
       <c r="E3" t="n">
         <v>0.675904574</v>
       </c>
       <c r="F3" t="n">
-        <v>2.15087103843689</v>
+        <v>1.86379861831665</v>
       </c>
       <c r="G3" t="n">
-        <v>1.47496646443689</v>
+        <v>1.18789404431665</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>2.052312850952148</v>
+        <v>1.662627339363098</v>
       </c>
       <c r="J3" t="n">
-        <v>2.052312850952148</v>
+        <v>1.662627339363098</v>
       </c>
     </row>
     <row r="4">
@@ -6363,28 +6363,28 @@
         <v>2.546268592</v>
       </c>
       <c r="C4" t="n">
-        <v>1.590012788772583</v>
+        <v>2.054032564163208</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9562558032274171</v>
+        <v>0.4922360278367921</v>
       </c>
       <c r="E4" t="n">
         <v>0.49047412</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6851937174797058</v>
+        <v>1.054974913597107</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1947195974797058</v>
+        <v>0.5645007935971069</v>
       </c>
       <c r="H4" t="n">
         <v>0.521059036</v>
       </c>
       <c r="I4" t="n">
-        <v>0.5087978839874268</v>
+        <v>0.7916519641876221</v>
       </c>
       <c r="J4" t="n">
-        <v>0.01226115201257327</v>
+        <v>0.270592928187622</v>
       </c>
     </row>
     <row r="5">
@@ -6397,28 +6397,28 @@
         <v>10.66375011</v>
       </c>
       <c r="C5" t="n">
-        <v>3.480880975723267</v>
+        <v>4.242328643798828</v>
       </c>
       <c r="D5" t="n">
-        <v>7.182869134276734</v>
+        <v>6.421421466201172</v>
       </c>
       <c r="E5" t="n">
         <v>5.367750915</v>
       </c>
       <c r="F5" t="n">
-        <v>2.3523850440979</v>
+        <v>2.805562257766724</v>
       </c>
       <c r="G5" t="n">
-        <v>3.0153658709021</v>
+        <v>2.562188657233277</v>
       </c>
       <c r="H5" t="n">
         <v>0.899989776</v>
       </c>
       <c r="I5" t="n">
-        <v>0.2386967390775681</v>
+        <v>0.5151007175445557</v>
       </c>
       <c r="J5" t="n">
-        <v>0.6612930369224319</v>
+        <v>0.3848890584554443</v>
       </c>
     </row>
     <row r="6">
@@ -6431,28 +6431,28 @@
         <v>15.57953993</v>
       </c>
       <c r="C6" t="n">
-        <v>3.64106011390686</v>
+        <v>4.419394493103027</v>
       </c>
       <c r="D6" t="n">
-        <v>11.93847981609314</v>
+        <v>11.16014543689697</v>
       </c>
       <c r="E6" t="n">
         <v>7.136655409</v>
       </c>
       <c r="F6" t="n">
-        <v>2.30732798576355</v>
+        <v>2.777554750442505</v>
       </c>
       <c r="G6" t="n">
-        <v>4.82932742323645</v>
+        <v>4.359100658557495</v>
       </c>
       <c r="H6" t="n">
         <v>0.923829666</v>
       </c>
       <c r="I6" t="n">
-        <v>0.1031937748193741</v>
+        <v>0.3644145727157593</v>
       </c>
       <c r="J6" t="n">
-        <v>0.820635891180626</v>
+        <v>0.5594150932842408</v>
       </c>
     </row>
     <row r="7">
@@ -6465,28 +6465,28 @@
         <v>1.019390288</v>
       </c>
       <c r="C7" t="n">
-        <v>2.013847351074219</v>
+        <v>2.330676794052124</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9944570630742187</v>
+        <v>1.311286506052124</v>
       </c>
       <c r="E7" t="n">
         <v>3.481328281</v>
       </c>
       <c r="F7" t="n">
-        <v>2.919358491897583</v>
+        <v>3.237976789474487</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5619697891024171</v>
+        <v>0.2433514915255128</v>
       </c>
       <c r="H7" t="n">
         <v>0.617193099</v>
       </c>
       <c r="I7" t="n">
-        <v>0.5008716583251953</v>
+        <v>0.4918133616447449</v>
       </c>
       <c r="J7" t="n">
-        <v>0.1163214406748047</v>
+        <v>0.1253797373552551</v>
       </c>
     </row>
     <row r="8">
@@ -6499,28 +6499,28 @@
         <v>18.58728802</v>
       </c>
       <c r="C8" t="n">
-        <v>16.35537910461426</v>
+        <v>15.86813163757324</v>
       </c>
       <c r="D8" t="n">
-        <v>2.231908915385741</v>
+        <v>2.719156382426757</v>
       </c>
       <c r="E8" t="n">
         <v>7.723795356</v>
       </c>
       <c r="F8" t="n">
-        <v>6.601923942565918</v>
+        <v>5.914060592651367</v>
       </c>
       <c r="G8" t="n">
-        <v>1.121871413434082</v>
+        <v>1.809734763348633</v>
       </c>
       <c r="H8" t="n">
         <v>1.139338063</v>
       </c>
       <c r="I8" t="n">
-        <v>0.7546231150627136</v>
+        <v>0.7233356237411499</v>
       </c>
       <c r="J8" t="n">
-        <v>0.3847149479372864</v>
+        <v>0.4160024392588502</v>
       </c>
     </row>
     <row r="9">
@@ -6533,28 +6533,28 @@
         <v>6.151374632</v>
       </c>
       <c r="C9" t="n">
-        <v>4.085438251495361</v>
+        <v>4.361367225646973</v>
       </c>
       <c r="D9" t="n">
-        <v>2.065936380504638</v>
+        <v>1.790007406353027</v>
       </c>
       <c r="E9" t="n">
         <v>1.201903721</v>
       </c>
       <c r="F9" t="n">
-        <v>0.7122712731361389</v>
+        <v>1.004542469978333</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4896324478638612</v>
+        <v>0.1973612510216676</v>
       </c>
       <c r="H9" t="n">
         <v>1.487273197</v>
       </c>
       <c r="I9" t="n">
-        <v>2.848731994628906</v>
+        <v>2.882237195968628</v>
       </c>
       <c r="J9" t="n">
-        <v>1.361458797628906</v>
+        <v>1.394963998968628</v>
       </c>
     </row>
     <row r="10">
@@ -6567,28 +6567,28 @@
         <v>12.36649696</v>
       </c>
       <c r="C10" t="n">
-        <v>10.40627384185791</v>
+        <v>9.265346527099609</v>
       </c>
       <c r="D10" t="n">
-        <v>1.960223118142089</v>
+        <v>3.10115043290039</v>
       </c>
       <c r="E10" t="n">
         <v>2.524540508</v>
       </c>
       <c r="F10" t="n">
-        <v>1.978761553764343</v>
+        <v>1.8836590051651</v>
       </c>
       <c r="G10" t="n">
-        <v>0.5457789542356566</v>
+        <v>0.6408815028348998</v>
       </c>
       <c r="H10" t="n">
         <v>1.956480352</v>
       </c>
       <c r="I10" t="n">
-        <v>3.814637660980225</v>
+        <v>2.969884157180786</v>
       </c>
       <c r="J10" t="n">
-        <v>1.858157308980225</v>
+        <v>1.013403805180786</v>
       </c>
     </row>
     <row r="11">
@@ -6601,28 +6601,28 @@
         <v>0.974600892</v>
       </c>
       <c r="C11" t="n">
-        <v>1.731987953186035</v>
+        <v>2.110862016677856</v>
       </c>
       <c r="D11" t="n">
-        <v>0.7573870611860352</v>
+        <v>1.136261124677856</v>
       </c>
       <c r="E11" t="n">
         <v>0.393635915</v>
       </c>
       <c r="F11" t="n">
-        <v>1.130110025405884</v>
+        <v>1.530386924743652</v>
       </c>
       <c r="G11" t="n">
-        <v>0.7364741104058838</v>
+        <v>1.136751009743652</v>
       </c>
       <c r="H11" t="n">
         <v>0.160959039</v>
       </c>
       <c r="I11" t="n">
-        <v>0.3677033185958862</v>
+        <v>0.4985709190368652</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2067442795958862</v>
+        <v>0.3376118800368653</v>
       </c>
     </row>
     <row r="12">
@@ -6635,28 +6635,28 @@
         <v>0.785805872</v>
       </c>
       <c r="C12" t="n">
-        <v>1.444767117500305</v>
+        <v>1.530370354652405</v>
       </c>
       <c r="D12" t="n">
-        <v>0.6589612455003052</v>
+        <v>0.7445644826524048</v>
       </c>
       <c r="E12" t="n">
         <v>0.692475215</v>
       </c>
       <c r="F12" t="n">
-        <v>1.21329391002655</v>
+        <v>1.573949337005615</v>
       </c>
       <c r="G12" t="n">
-        <v>0.5208186950265503</v>
+        <v>0.8814741220056153</v>
       </c>
       <c r="H12" t="n">
         <v>0.195450855</v>
       </c>
       <c r="I12" t="n">
-        <v>0.3128553628921509</v>
+        <v>0.2625041604042053</v>
       </c>
       <c r="J12" t="n">
-        <v>0.1174045078921509</v>
+        <v>0.06705330540420532</v>
       </c>
     </row>
     <row r="13">
@@ -6669,28 +6669,28 @@
         <v>1.0344302</v>
       </c>
       <c r="C13" t="n">
-        <v>2.025751352310181</v>
+        <v>2.256744861602783</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9913211523101806</v>
+        <v>1.222314661602783</v>
       </c>
       <c r="E13" t="n">
         <v>3.016436227</v>
       </c>
       <c r="F13" t="n">
-        <v>2.585455894470215</v>
+        <v>2.960287809371948</v>
       </c>
       <c r="G13" t="n">
-        <v>0.430980332529785</v>
+        <v>0.05614841762805156</v>
       </c>
       <c r="H13" t="n">
         <v>0.408449459</v>
       </c>
       <c r="I13" t="n">
-        <v>0.3083294034004211</v>
+        <v>0.2946279048919678</v>
       </c>
       <c r="J13" t="n">
-        <v>0.1001200555995789</v>
+        <v>0.1138215541080322</v>
       </c>
     </row>
     <row r="14">
@@ -6703,28 +6703,28 @@
         <v>61.8038557</v>
       </c>
       <c r="C14" t="n">
-        <v>57.56928253173828</v>
+        <v>53.59357070922852</v>
       </c>
       <c r="D14" t="n">
-        <v>4.234573168261718</v>
+        <v>8.210284990771484</v>
       </c>
       <c r="E14" t="n">
         <v>25.01149768</v>
       </c>
       <c r="F14" t="n">
-        <v>21.89504623413086</v>
+        <v>18.53630638122559</v>
       </c>
       <c r="G14" t="n">
-        <v>3.116451445869142</v>
+        <v>6.475191298774416</v>
       </c>
       <c r="H14" t="n">
         <v>3.730481208</v>
       </c>
       <c r="I14" t="n">
-        <v>4.003339767456055</v>
+        <v>3.57302713394165</v>
       </c>
       <c r="J14" t="n">
-        <v>0.2728585594560546</v>
+        <v>0.1574540740583497</v>
       </c>
     </row>
     <row r="15">
@@ -6737,28 +6737,28 @@
         <v>2.518653476</v>
       </c>
       <c r="C15" t="n">
-        <v>1.690682172775269</v>
+        <v>2.169328927993774</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8279713032247313</v>
+        <v>0.3493245480062255</v>
       </c>
       <c r="E15" t="n">
         <v>0.66817386</v>
       </c>
       <c r="F15" t="n">
-        <v>0.8464617729187012</v>
+        <v>1.241965532302856</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1782879129187012</v>
+        <v>0.5737916723028564</v>
       </c>
       <c r="H15" t="n">
         <v>0.5032910390000001</v>
       </c>
       <c r="I15" t="n">
-        <v>0.4966763854026794</v>
+        <v>0.7602269649505615</v>
       </c>
       <c r="J15" t="n">
-        <v>0.006614653597320608</v>
+        <v>0.2569359259505615</v>
       </c>
     </row>
     <row r="16">
@@ -6771,28 +6771,28 @@
         <v>1.006196007</v>
       </c>
       <c r="C16" t="n">
-        <v>1.754834055900574</v>
+        <v>2.101152896881104</v>
       </c>
       <c r="D16" t="n">
-        <v>0.7486380489005737</v>
+        <v>1.094956889881104</v>
       </c>
       <c r="E16" t="n">
         <v>0.464787932</v>
       </c>
       <c r="F16" t="n">
-        <v>1.175041198730469</v>
+        <v>1.580263376235962</v>
       </c>
       <c r="G16" t="n">
-        <v>0.7102532667304687</v>
+        <v>1.115475444235962</v>
       </c>
       <c r="H16" t="n">
         <v>0.186124482</v>
       </c>
       <c r="I16" t="n">
-        <v>0.2999914884567261</v>
+        <v>0.3755123615264893</v>
       </c>
       <c r="J16" t="n">
-        <v>0.1138670064567261</v>
+        <v>0.1893878795264893</v>
       </c>
     </row>
     <row r="17">
@@ -6805,28 +6805,28 @@
         <v>2.380706892</v>
       </c>
       <c r="C17" t="n">
-        <v>1.90115213394165</v>
+        <v>2.506531238555908</v>
       </c>
       <c r="D17" t="n">
-        <v>0.4795547580583497</v>
+        <v>0.1258243465559081</v>
       </c>
       <c r="E17" t="n">
         <v>1.708296635</v>
       </c>
       <c r="F17" t="n">
-        <v>1.771840333938599</v>
+        <v>2.050143003463745</v>
       </c>
       <c r="G17" t="n">
-        <v>0.06354369893859868</v>
+        <v>0.3418463684637452</v>
       </c>
       <c r="H17" t="n">
         <v>0.8350595240000001</v>
       </c>
       <c r="I17" t="n">
-        <v>0.9718776345252991</v>
+        <v>1.240594744682312</v>
       </c>
       <c r="J17" t="n">
-        <v>0.136818110525299</v>
+        <v>0.405535220682312</v>
       </c>
     </row>
     <row r="18">
@@ -6839,28 +6839,28 @@
         <v>1.78069478</v>
       </c>
       <c r="C18" t="n">
-        <v>2.591815233230591</v>
+        <v>3.325734853744507</v>
       </c>
       <c r="D18" t="n">
-        <v>0.8111204532305909</v>
+        <v>1.545040073744507</v>
       </c>
       <c r="E18" t="n">
         <v>0.505519908</v>
       </c>
       <c r="F18" t="n">
-        <v>1.207934737205505</v>
+        <v>1.721148252487183</v>
       </c>
       <c r="G18" t="n">
-        <v>0.7024148292055054</v>
+        <v>1.215628344487182</v>
       </c>
       <c r="H18" t="n">
         <v>0.176196273</v>
       </c>
       <c r="I18" t="n">
-        <v>0.3468466997146606</v>
+        <v>0.5981664061546326</v>
       </c>
       <c r="J18" t="n">
-        <v>0.1706504267146607</v>
+        <v>0.4219701331546326</v>
       </c>
     </row>
     <row r="19">
@@ -6873,28 +6873,28 @@
         <v>3.711818396</v>
       </c>
       <c r="C19" t="n">
-        <v>3.006704330444336</v>
+        <v>2.547013998031616</v>
       </c>
       <c r="D19" t="n">
-        <v>0.705114065555664</v>
+        <v>1.164804397968384</v>
       </c>
       <c r="E19" t="n">
         <v>5.914797556</v>
       </c>
       <c r="F19" t="n">
-        <v>5.665797233581543</v>
+        <v>5.844404220581055</v>
       </c>
       <c r="G19" t="n">
-        <v>0.2490003224184569</v>
+        <v>0.07039333541894521</v>
       </c>
       <c r="H19" t="n">
         <v>3.160119003</v>
       </c>
       <c r="I19" t="n">
-        <v>5.656315803527832</v>
+        <v>5.191498756408691</v>
       </c>
       <c r="J19" t="n">
-        <v>2.496196800527832</v>
+        <v>2.031379753408691</v>
       </c>
     </row>
     <row r="20">
@@ -6907,28 +6907,28 @@
         <v>1.10214478</v>
       </c>
       <c r="C20" t="n">
-        <v>2.811300992965698</v>
+        <v>3.466354131698608</v>
       </c>
       <c r="D20" t="n">
-        <v>1.709156212965698</v>
+        <v>2.364209351698609</v>
       </c>
       <c r="E20" t="n">
         <v>0.797685387</v>
       </c>
       <c r="F20" t="n">
-        <v>2.353917360305786</v>
+        <v>2.780101776123047</v>
       </c>
       <c r="G20" t="n">
-        <v>1.556231973305786</v>
+        <v>1.982416389123047</v>
       </c>
       <c r="H20" t="n">
         <v>0.149094864</v>
       </c>
       <c r="I20" t="n">
-        <v>0.2360158115625381</v>
+        <v>0.4389534592628479</v>
       </c>
       <c r="J20" t="n">
-        <v>0.08692094756253815</v>
+        <v>0.2898585952628479</v>
       </c>
     </row>
     <row r="21">
@@ -6941,28 +6941,28 @@
         <v>81.05285287</v>
       </c>
       <c r="C21" t="n">
-        <v>86.48673248291016</v>
+        <v>80.08550262451172</v>
       </c>
       <c r="D21" t="n">
-        <v>5.433879612910161</v>
+        <v>0.9673502454882765</v>
       </c>
       <c r="E21" t="n">
         <v>35.78282597</v>
       </c>
       <c r="F21" t="n">
-        <v>35.82675170898438</v>
+        <v>31.33637619018555</v>
       </c>
       <c r="G21" t="n">
-        <v>0.04392573898437746</v>
+        <v>4.446449779814451</v>
       </c>
       <c r="H21" t="n">
         <v>4.612928547</v>
       </c>
       <c r="I21" t="n">
-        <v>5.120907783508301</v>
+        <v>4.830312728881836</v>
       </c>
       <c r="J21" t="n">
-        <v>0.5079792365083007</v>
+        <v>0.2173841818818358</v>
       </c>
     </row>
     <row r="22">
@@ -6975,28 +6975,28 @@
         <v>0.469325038</v>
       </c>
       <c r="C22" t="n">
-        <v>1.126173734664917</v>
+        <v>1.569989681243896</v>
       </c>
       <c r="D22" t="n">
-        <v>0.656848696664917</v>
+        <v>1.100664643243896</v>
       </c>
       <c r="E22" t="n">
         <v>0.321616579</v>
       </c>
       <c r="F22" t="n">
-        <v>1.304885149002075</v>
+        <v>1.520691633224487</v>
       </c>
       <c r="G22" t="n">
-        <v>0.9832685700020751</v>
+        <v>1.199075054224487</v>
       </c>
       <c r="H22" t="n">
         <v>0.34214243</v>
       </c>
       <c r="I22" t="n">
-        <v>1.589310765266418</v>
+        <v>2.080085039138794</v>
       </c>
       <c r="J22" t="n">
-        <v>1.247168335266418</v>
+        <v>1.737942609138794</v>
       </c>
     </row>
     <row r="23">
@@ -7009,28 +7009,28 @@
         <v>148.5633238</v>
       </c>
       <c r="C23" t="n">
-        <v>165.0450744628906</v>
+        <v>151.488037109375</v>
       </c>
       <c r="D23" t="n">
-        <v>16.48175066289062</v>
+        <v>2.924713309374994</v>
       </c>
       <c r="E23" t="n">
         <v>77.75262948</v>
       </c>
       <c r="F23" t="n">
-        <v>84.67376708984375</v>
+        <v>76.93002319335938</v>
       </c>
       <c r="G23" t="n">
-        <v>6.921137609843754</v>
+        <v>0.822606286640621</v>
       </c>
       <c r="H23" t="n">
         <v>8.3128054</v>
       </c>
       <c r="I23" t="n">
-        <v>6.685192584991455</v>
+        <v>7.838691234588623</v>
       </c>
       <c r="J23" t="n">
-        <v>1.627612815008545</v>
+        <v>0.4741141654113772</v>
       </c>
     </row>
     <row r="24">
@@ -7043,28 +7043,28 @@
         <v>2.139793073</v>
       </c>
       <c r="C24" t="n">
-        <v>1.645090818405151</v>
+        <v>2.1812584400177</v>
       </c>
       <c r="D24" t="n">
-        <v>0.4947022545948485</v>
+        <v>0.04146536701770032</v>
       </c>
       <c r="E24" t="n">
         <v>0.635588045</v>
       </c>
       <c r="F24" t="n">
-        <v>0.8718785643577576</v>
+        <v>1.201701521873474</v>
       </c>
       <c r="G24" t="n">
-        <v>0.2362905193577576</v>
+        <v>0.5661134768734741</v>
       </c>
       <c r="H24" t="n">
         <v>0.603471757</v>
       </c>
       <c r="I24" t="n">
-        <v>0.9275170564651489</v>
+        <v>1.322614312171936</v>
       </c>
       <c r="J24" t="n">
-        <v>0.3240452994651489</v>
+        <v>0.719142555171936</v>
       </c>
     </row>
     <row r="25">
@@ -7077,28 +7077,28 @@
         <v>22.11509533</v>
       </c>
       <c r="C25" t="n">
-        <v>26.94645690917969</v>
+        <v>24.87978172302246</v>
       </c>
       <c r="D25" t="n">
-        <v>4.831361579179688</v>
+        <v>2.764686393022462</v>
       </c>
       <c r="E25" t="n">
         <v>7.78555279</v>
       </c>
       <c r="F25" t="n">
-        <v>9.140545845031738</v>
+        <v>7.463892459869385</v>
       </c>
       <c r="G25" t="n">
-        <v>1.354993055031739</v>
+        <v>0.3216603301306149</v>
       </c>
       <c r="H25" t="n">
         <v>1.185972621</v>
       </c>
       <c r="I25" t="n">
-        <v>1.702297210693359</v>
+        <v>1.29400098323822</v>
       </c>
       <c r="J25" t="n">
-        <v>0.5163245896933595</v>
+        <v>0.1080283622382203</v>
       </c>
     </row>
     <row r="26">
@@ -7111,28 +7111,28 @@
         <v>18.64251276</v>
       </c>
       <c r="C26" t="n">
-        <v>14.53476810455322</v>
+        <v>14.4576416015625</v>
       </c>
       <c r="D26" t="n">
-        <v>4.107744655446776</v>
+        <v>4.184871158437499</v>
       </c>
       <c r="E26" t="n">
         <v>5.905318651</v>
       </c>
       <c r="F26" t="n">
-        <v>4.985452651977539</v>
+        <v>4.483814716339111</v>
       </c>
       <c r="G26" t="n">
-        <v>0.9198659990224609</v>
+        <v>1.421503934660889</v>
       </c>
       <c r="H26" t="n">
         <v>1.306022159</v>
       </c>
       <c r="I26" t="n">
-        <v>1.08689296245575</v>
+        <v>0.933152437210083</v>
       </c>
       <c r="J26" t="n">
-        <v>0.2191291965442506</v>
+        <v>0.3728697217899171</v>
       </c>
     </row>
     <row r="27">
@@ -7145,28 +7145,28 @@
         <v>1.112044379</v>
       </c>
       <c r="C27" t="n">
-        <v>2.293047904968262</v>
+        <v>2.814109563827515</v>
       </c>
       <c r="D27" t="n">
-        <v>1.181003525968262</v>
+        <v>1.702065184827515</v>
       </c>
       <c r="E27" t="n">
         <v>1.472169653</v>
       </c>
       <c r="F27" t="n">
-        <v>2.715330362319946</v>
+        <v>3.054393529891968</v>
       </c>
       <c r="G27" t="n">
-        <v>1.243160709319946</v>
+        <v>1.582223876891968</v>
       </c>
       <c r="H27" t="n">
         <v>0.310931952</v>
       </c>
       <c r="I27" t="n">
-        <v>0.4963430762290955</v>
+        <v>0.6440065503120422</v>
       </c>
       <c r="J27" t="n">
-        <v>0.1854111242290954</v>
+        <v>0.3330745983120422</v>
       </c>
     </row>
     <row r="28">
@@ -7179,28 +7179,28 @@
         <v>1.00422288</v>
       </c>
       <c r="C28" t="n">
-        <v>5.167090892791748</v>
+        <v>5.776369571685791</v>
       </c>
       <c r="D28" t="n">
-        <v>4.162868012791748</v>
+        <v>4.772146691685791</v>
       </c>
       <c r="E28" t="n">
         <v>0.86154519</v>
       </c>
       <c r="F28" t="n">
-        <v>4.611931800842285</v>
+        <v>4.946385860443115</v>
       </c>
       <c r="G28" t="n">
-        <v>3.750386610842285</v>
+        <v>4.084840670443115</v>
       </c>
       <c r="H28" t="n">
         <v>0.086345371</v>
       </c>
       <c r="I28" t="n">
-        <v>-0.0267719179391861</v>
+        <v>0.0886867567896843</v>
       </c>
       <c r="J28" t="n">
-        <v>0.1131172889391861</v>
+        <v>0.002341385789684292</v>
       </c>
     </row>
     <row r="29">
@@ -7213,28 +7213,28 @@
         <v>8.949079931</v>
       </c>
       <c r="C29" t="n">
-        <v>2.794551134109497</v>
+        <v>3.456521272659302</v>
       </c>
       <c r="D29" t="n">
-        <v>6.154528796890503</v>
+        <v>5.492558658340698</v>
       </c>
       <c r="E29" t="n">
         <v>5.734039206</v>
       </c>
       <c r="F29" t="n">
-        <v>2.249882221221924</v>
+        <v>2.681339979171753</v>
       </c>
       <c r="G29" t="n">
-        <v>3.484156984778076</v>
+        <v>3.052699226828247</v>
       </c>
       <c r="H29" t="n">
         <v>0.847154045</v>
       </c>
       <c r="I29" t="n">
-        <v>0.2085471153259277</v>
+        <v>0.400057315826416</v>
       </c>
       <c r="J29" t="n">
-        <v>0.6386069296740723</v>
+        <v>0.447096729173584</v>
       </c>
     </row>
     <row r="30">
@@ -7247,28 +7247,28 @@
         <v>3.861971089</v>
       </c>
       <c r="C30" t="n">
-        <v>6.04601526260376</v>
+        <v>6.788624286651611</v>
       </c>
       <c r="D30" t="n">
-        <v>2.18404417360376</v>
+        <v>2.926653197651611</v>
       </c>
       <c r="E30" t="n">
         <v>2.16573855</v>
       </c>
       <c r="F30" t="n">
-        <v>2.254735946655273</v>
+        <v>2.459293842315674</v>
       </c>
       <c r="G30" t="n">
-        <v>0.08899739665527351</v>
+        <v>0.2935552923156739</v>
       </c>
       <c r="H30" t="n">
         <v>1.026875013</v>
       </c>
       <c r="I30" t="n">
-        <v>0.9835784435272217</v>
+        <v>1.221905469894409</v>
       </c>
       <c r="J30" t="n">
-        <v>0.04329656947277827</v>
+        <v>0.1950304568944092</v>
       </c>
     </row>
     <row r="31">
@@ -7281,28 +7281,28 @@
         <v>2.694129305</v>
       </c>
       <c r="C31" t="n">
-        <v>7.042696475982666</v>
+        <v>6.326809883117676</v>
       </c>
       <c r="D31" t="n">
-        <v>4.348567170982665</v>
+        <v>3.632680578117676</v>
       </c>
       <c r="E31" t="n">
         <v>8.998579747999999</v>
       </c>
       <c r="F31" t="n">
-        <v>14.48710823059082</v>
+        <v>13.50008583068848</v>
       </c>
       <c r="G31" t="n">
-        <v>5.488528482590821</v>
+        <v>4.501506082688477</v>
       </c>
       <c r="H31" t="n">
         <v>1.07537871</v>
       </c>
       <c r="I31" t="n">
-        <v>2.68515157699585</v>
+        <v>2.174927234649658</v>
       </c>
       <c r="J31" t="n">
-        <v>1.60977286699585</v>
+        <v>1.099548524649658</v>
       </c>
     </row>
     <row r="32">
@@ -7315,28 +7315,28 @@
         <v>9.584904244000001</v>
       </c>
       <c r="C32" t="n">
-        <v>2.217966794967651</v>
+        <v>2.728539228439331</v>
       </c>
       <c r="D32" t="n">
-        <v>7.366937449032349</v>
+        <v>6.856365015560669</v>
       </c>
       <c r="E32" t="n">
         <v>28.10562387</v>
       </c>
       <c r="F32" t="n">
-        <v>4.94398307800293</v>
+        <v>5.06915283203125</v>
       </c>
       <c r="G32" t="n">
-        <v>23.16164079199707</v>
+        <v>23.03647103796875</v>
       </c>
       <c r="H32" t="n">
         <v>7.878814553</v>
       </c>
       <c r="I32" t="n">
-        <v>1.777146816253662</v>
+        <v>1.975358963012695</v>
       </c>
       <c r="J32" t="n">
-        <v>6.101667736746338</v>
+        <v>5.903455589987304</v>
       </c>
     </row>
     <row r="33">
@@ -7349,28 +7349,28 @@
         <v>22.11264958</v>
       </c>
       <c r="C33" t="n">
-        <v>18.12860107421875</v>
+        <v>17.22923469543457</v>
       </c>
       <c r="D33" t="n">
-        <v>3.984048505781249</v>
+        <v>4.883414884565429</v>
       </c>
       <c r="E33" t="n">
         <v>7.102343521</v>
       </c>
       <c r="F33" t="n">
-        <v>5.975821495056152</v>
+        <v>5.166049003601074</v>
       </c>
       <c r="G33" t="n">
-        <v>1.126522025943848</v>
+        <v>1.936294517398926</v>
       </c>
       <c r="H33" t="n">
         <v>1.625014611</v>
       </c>
       <c r="I33" t="n">
-        <v>1.521459579467773</v>
+        <v>1.104485034942627</v>
       </c>
       <c r="J33" t="n">
-        <v>0.1035550315322267</v>
+        <v>0.5205295760573732</v>
       </c>
     </row>
   </sheetData>

</xml_diff>